<commit_message>
Update latest model tuning
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
-    <sheet name="new" sheetId="3" r:id="rId1"/>
+    <sheet name="prioritize induction" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -205,6 +205,66 @@
   </si>
   <si>
     <t>tau_fac</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -597,10 +657,10 @@
   <dimension ref="A1:CV58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -636,6 +696,51 @@
       </c>
       <c r="F1" t="s">
         <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" t="s">
+        <v>62</v>
       </c>
       <c r="BA1" s="4"/>
       <c r="BB1" s="4"/>
@@ -695,6 +800,48 @@
       <c r="F3" s="4">
         <v>1.2</v>
       </c>
+      <c r="G3" s="4">
+        <v>1.58</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1.24</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1.21</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1.69</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1.69</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="N3" s="4">
+        <v>1.33</v>
+      </c>
+      <c r="O3" s="4">
+        <v>1.26</v>
+      </c>
+      <c r="P3" s="4">
+        <v>1.33</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>1.33</v>
+      </c>
+      <c r="R3" s="4">
+        <v>1.27</v>
+      </c>
+      <c r="S3" s="4">
+        <v>1.35</v>
+      </c>
+      <c r="T3" s="4">
+        <v>1.32</v>
+      </c>
       <c r="BH3" s="7"/>
       <c r="BM3" s="7"/>
       <c r="BQ3" s="7"/>
@@ -715,6 +862,48 @@
       <c r="F4" s="4">
         <v>0.98299999999999998</v>
       </c>
+      <c r="G4" s="4">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1.04</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="R4" s="4">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="S4" s="4">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="T4" s="4">
+        <v>0.83299999999999996</v>
+      </c>
       <c r="BH4" s="7"/>
       <c r="BM4" s="7"/>
       <c r="BQ4" s="7"/>
@@ -735,6 +924,48 @@
       <c r="F5" s="4">
         <v>0.30399999999999999</v>
       </c>
+      <c r="G5" s="4">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.371</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.81</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1.19</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1.99</v>
+      </c>
+      <c r="L5" s="4">
+        <v>2.09</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1.32</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1.21</v>
+      </c>
+      <c r="O5" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="P5" s="4">
+        <v>2.42</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>2.62</v>
+      </c>
+      <c r="R5" s="4">
+        <v>1.21</v>
+      </c>
+      <c r="S5" s="4">
+        <v>2.15</v>
+      </c>
+      <c r="T5" s="4">
+        <v>2.37</v>
+      </c>
       <c r="BH5" s="7"/>
       <c r="BM5" s="7"/>
       <c r="BQ5" s="7"/>
@@ -752,6 +983,48 @@
       <c r="F6" s="4">
         <v>0.48299999999999998</v>
       </c>
+      <c r="G6" s="4">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0.88</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1.41</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1.43</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1.19</v>
+      </c>
+      <c r="N6" s="4">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="O6" s="4">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="P6" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>1.69</v>
+      </c>
+      <c r="R6" s="4">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="S6" s="4">
+        <v>1.47</v>
+      </c>
+      <c r="T6" s="4">
+        <v>1.56</v>
+      </c>
       <c r="BH6" s="7"/>
       <c r="BM6" s="7"/>
       <c r="BQ6" s="7"/>
@@ -772,6 +1045,48 @@
       <c r="F7" s="4">
         <v>1.69</v>
       </c>
+      <c r="G7" s="4">
+        <v>3.26</v>
+      </c>
+      <c r="H7" s="4">
+        <v>4.58</v>
+      </c>
+      <c r="I7" s="4">
+        <v>3.97</v>
+      </c>
+      <c r="J7" s="4">
+        <v>4.04</v>
+      </c>
+      <c r="K7" s="4">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="L7" s="4">
+        <v>4.01</v>
+      </c>
+      <c r="M7" s="4">
+        <v>3.38</v>
+      </c>
+      <c r="N7" s="4">
+        <v>3.59</v>
+      </c>
+      <c r="O7" s="4">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="P7" s="4">
+        <v>3.58</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="R7" s="4">
+        <v>4.28</v>
+      </c>
+      <c r="S7" s="4">
+        <v>3.99</v>
+      </c>
+      <c r="T7" s="4">
+        <v>3.75</v>
+      </c>
       <c r="BH7" s="7"/>
       <c r="BM7" s="7"/>
       <c r="BQ7" s="7"/>
@@ -789,6 +1104,48 @@
       <c r="F8" s="4">
         <v>3.85</v>
       </c>
+      <c r="G8" s="4">
+        <v>5.55</v>
+      </c>
+      <c r="H8" s="4">
+        <v>6.65</v>
+      </c>
+      <c r="I8" s="4">
+        <v>6.16</v>
+      </c>
+      <c r="J8" s="4">
+        <v>6.19</v>
+      </c>
+      <c r="K8" s="4">
+        <v>6.22</v>
+      </c>
+      <c r="L8" s="4">
+        <v>6.17</v>
+      </c>
+      <c r="M8" s="4">
+        <v>5.55</v>
+      </c>
+      <c r="N8" s="4">
+        <v>5.68</v>
+      </c>
+      <c r="O8" s="4">
+        <v>6.08</v>
+      </c>
+      <c r="P8" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>5.58</v>
+      </c>
+      <c r="R8" s="4">
+        <v>6.19</v>
+      </c>
+      <c r="S8" s="4">
+        <v>5.97</v>
+      </c>
+      <c r="T8" s="4">
+        <v>5.83</v>
+      </c>
       <c r="BH8" s="7"/>
       <c r="BM8" s="7"/>
       <c r="BQ8" s="7"/>
@@ -809,6 +1166,48 @@
       <c r="F9" s="4">
         <v>4.21</v>
       </c>
+      <c r="G9" s="4">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="H9" s="4">
+        <v>3.7699999999999997E-2</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="J9" s="4">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1.77</v>
+      </c>
+      <c r="M9" s="4">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="N9" s="4">
+        <v>2.23</v>
+      </c>
+      <c r="O9" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="P9" s="4">
+        <v>7.91</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="R9" s="4">
+        <v>1.43</v>
+      </c>
+      <c r="S9" s="4">
+        <v>6.35</v>
+      </c>
+      <c r="T9" s="4">
+        <v>7.36</v>
+      </c>
       <c r="BH9" s="7"/>
       <c r="BM9" s="7"/>
       <c r="BQ9" s="7"/>
@@ -826,6 +1225,48 @@
       <c r="F10" s="4">
         <v>5.15</v>
       </c>
+      <c r="G10" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1.24</v>
+      </c>
+      <c r="J10" s="4">
+        <v>1.17</v>
+      </c>
+      <c r="K10" s="4">
+        <v>2.33</v>
+      </c>
+      <c r="L10" s="4">
+        <v>2.39</v>
+      </c>
+      <c r="M10" s="4">
+        <v>2.54</v>
+      </c>
+      <c r="N10" s="4">
+        <v>2.17</v>
+      </c>
+      <c r="O10" s="4">
+        <v>1.79</v>
+      </c>
+      <c r="P10" s="4">
+        <v>5.56</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>5.99</v>
+      </c>
+      <c r="R10" s="4">
+        <v>1.49</v>
+      </c>
+      <c r="S10" s="4">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="T10" s="4">
+        <v>5.08</v>
+      </c>
       <c r="BH10" s="7"/>
       <c r="BM10" s="7"/>
       <c r="BQ10" s="7"/>
@@ -862,6 +1303,12 @@
       <c r="G17" s="4">
         <v>16</v>
       </c>
+      <c r="H17" s="4">
+        <v>15</v>
+      </c>
+      <c r="N17" s="4">
+        <v>20</v>
+      </c>
       <c r="CI17"/>
       <c r="CM17" s="4"/>
     </row>
@@ -878,6 +1325,18 @@
       <c r="G18" s="4">
         <v>30</v>
       </c>
+      <c r="H18" s="4">
+        <v>40</v>
+      </c>
+      <c r="I18" s="4">
+        <v>50</v>
+      </c>
+      <c r="J18" s="4">
+        <v>60</v>
+      </c>
+      <c r="O18" s="4">
+        <v>66</v>
+      </c>
       <c r="CM18" s="4"/>
     </row>
     <row r="19" spans="1:92">
@@ -893,6 +1352,24 @@
       <c r="G19" s="4">
         <v>5</v>
       </c>
+      <c r="H19" s="4">
+        <v>6</v>
+      </c>
+      <c r="I19" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="M19" s="4">
+        <v>5</v>
+      </c>
+      <c r="O19" s="4">
+        <v>5.3</v>
+      </c>
+      <c r="R19" s="4">
+        <v>5</v>
+      </c>
+      <c r="U19" s="4">
+        <v>4</v>
+      </c>
       <c r="CM19" s="4"/>
       <c r="CN19" s="4"/>
     </row>
@@ -909,6 +1386,24 @@
       <c r="G20" s="4">
         <v>1</v>
       </c>
+      <c r="H20" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="N20" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="O20" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="R20" s="4">
+        <v>0.1</v>
+      </c>
       <c r="CM20" s="4"/>
     </row>
     <row r="21" spans="1:92">
@@ -978,6 +1473,12 @@
       <c r="D26" s="6">
         <v>3.6</v>
       </c>
+      <c r="M26" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="U26" s="4">
+        <v>7.2</v>
+      </c>
       <c r="CM26" s="4"/>
     </row>
     <row r="27" spans="1:92">
@@ -990,6 +1491,12 @@
       <c r="D27" s="6">
         <v>1.65</v>
       </c>
+      <c r="M27" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="U27" s="4">
+        <v>3.3</v>
+      </c>
       <c r="CM27" s="4"/>
     </row>
     <row r="28" spans="1:92">
@@ -1002,6 +1509,9 @@
       <c r="D28" s="6">
         <v>0.12</v>
       </c>
+      <c r="M28" s="4">
+        <v>0.18</v>
+      </c>
       <c r="CM28" s="4"/>
     </row>
     <row r="29" spans="1:92">
@@ -1014,6 +1524,9 @@
       <c r="D29" s="6">
         <v>0.6</v>
       </c>
+      <c r="M29" s="4">
+        <v>0.89999999999999991</v>
+      </c>
       <c r="CM29" s="4"/>
     </row>
     <row r="30" spans="1:92">
@@ -1074,6 +1587,9 @@
       <c r="D34" s="6">
         <v>8.5</v>
       </c>
+      <c r="R34" s="4">
+        <v>6.8000000000000007</v>
+      </c>
       <c r="CM34" s="4"/>
     </row>
     <row r="35" spans="1:91">
@@ -1086,6 +1602,12 @@
       <c r="D35" s="6">
         <v>6</v>
       </c>
+      <c r="R35" s="4">
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="U35" s="4">
+        <v>6</v>
+      </c>
       <c r="CM35" s="4"/>
     </row>
     <row r="36" spans="1:91">
@@ -1098,6 +1620,12 @@
       <c r="D36" s="6">
         <v>1.6</v>
       </c>
+      <c r="R36" s="4">
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="U36" s="4">
+        <v>1.6</v>
+      </c>
       <c r="CM36" s="4"/>
     </row>
     <row r="37" spans="1:91">
@@ -1109,6 +1637,9 @@
       </c>
       <c r="D37" s="6">
         <v>0.6</v>
+      </c>
+      <c r="R37" s="4">
+        <v>0.44999999999999996</v>
       </c>
       <c r="CM37" s="4"/>
     </row>

</xml_diff>

<commit_message>
Switch to second set of synaptic parameters
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
-    <sheet name="prioritize induction" sheetId="3" r:id="rId1"/>
+    <sheet name="set 2" sheetId="5" r:id="rId1"/>
+    <sheet name="set 1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="70">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -265,6 +266,34 @@
   </si>
   <si>
     <t>baseline_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_13</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -654,13 +683,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="13.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="4" max="4" width="9" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" s="7">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="C10" s="7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="6">
+        <v>22</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6">
+        <v>70</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="6">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>0.152</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="D25" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="D26" s="6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29">
+        <v>0.11</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>1.79</v>
+      </c>
+      <c r="D30" s="6">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>6.67</v>
+      </c>
+      <c r="D31" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32">
+        <v>0.68</v>
+      </c>
+      <c r="D32" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="B33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="D33" s="6">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="B34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <v>1.87</v>
+      </c>
+      <c r="D34" s="6">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="B35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>1.56</v>
+      </c>
+      <c r="D35" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="B36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="D36" s="6">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="B37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37">
+        <v>0.432</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1.7000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="B40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="6">
+        <v>1.9000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="B43" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="B44" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="B45" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="B47" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="B48" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="B49" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="B54" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CV58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q30" sqref="Q30"/>
+      <selection pane="bottomRight" activeCell="Y17" sqref="Y17:Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -741,6 +1203,27 @@
       </c>
       <c r="U1" t="s">
         <v>62</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="W1" t="s">
+        <v>64</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>69</v>
       </c>
       <c r="BA1" s="4"/>
       <c r="BB1" s="4"/>
@@ -842,6 +1325,27 @@
       <c r="T3" s="4">
         <v>1.32</v>
       </c>
+      <c r="U3" s="4">
+        <v>1.27</v>
+      </c>
+      <c r="V3" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="W3" s="4">
+        <v>1.84</v>
+      </c>
+      <c r="X3" s="4">
+        <v>2.56</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>1.92</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>2.44</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>2.4500000000000002</v>
+      </c>
       <c r="BH3" s="7"/>
       <c r="BM3" s="7"/>
       <c r="BQ3" s="7"/>
@@ -904,6 +1408,27 @@
       <c r="T4" s="4">
         <v>0.83299999999999996</v>
       </c>
+      <c r="U4" s="4">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="V4" s="4">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="W4" s="4">
+        <v>1.28</v>
+      </c>
+      <c r="X4" s="4">
+        <v>1.46</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>1.24</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>1.18</v>
+      </c>
       <c r="BH4" s="7"/>
       <c r="BM4" s="7"/>
       <c r="BQ4" s="7"/>
@@ -966,6 +1491,27 @@
       <c r="T5" s="4">
         <v>2.37</v>
       </c>
+      <c r="U5" s="4">
+        <v>1.54</v>
+      </c>
+      <c r="V5" s="4">
+        <v>3.01</v>
+      </c>
+      <c r="W5" s="4">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="X5" s="4">
+        <v>1.07</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="Z5" s="4">
+        <v>1.64</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>2.0499999999999998</v>
+      </c>
       <c r="BH5" s="7"/>
       <c r="BM5" s="7"/>
       <c r="BQ5" s="7"/>
@@ -1025,6 +1571,27 @@
       <c r="T6" s="4">
         <v>1.56</v>
       </c>
+      <c r="U6" s="4">
+        <v>1.28</v>
+      </c>
+      <c r="V6" s="4">
+        <v>1.88</v>
+      </c>
+      <c r="W6" s="4">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="X6" s="4">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>1.05</v>
+      </c>
+      <c r="Z6" s="4">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="AA6" s="4">
+        <v>1.27</v>
+      </c>
       <c r="BH6" s="7"/>
       <c r="BM6" s="7"/>
       <c r="BQ6" s="7"/>
@@ -1087,6 +1654,27 @@
       <c r="T7" s="4">
         <v>3.75</v>
       </c>
+      <c r="U7" s="4">
+        <v>3.09</v>
+      </c>
+      <c r="V7" s="4">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="W7" s="4">
+        <v>4.72</v>
+      </c>
+      <c r="X7" s="4">
+        <v>5.64</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>4.18</v>
+      </c>
+      <c r="Z7" s="4">
+        <v>5.08</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>4.43</v>
+      </c>
       <c r="BH7" s="7"/>
       <c r="BM7" s="7"/>
       <c r="BQ7" s="7"/>
@@ -1146,6 +1734,27 @@
       <c r="T8" s="4">
         <v>5.83</v>
       </c>
+      <c r="U8" s="4">
+        <v>4.96</v>
+      </c>
+      <c r="V8" s="4">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="W8" s="4">
+        <v>5.66</v>
+      </c>
+      <c r="X8" s="4">
+        <v>5.87</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>4.51</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>4.71</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>4.57</v>
+      </c>
       <c r="BH8" s="7"/>
       <c r="BM8" s="7"/>
       <c r="BQ8" s="7"/>
@@ -1208,6 +1817,27 @@
       <c r="T9" s="4">
         <v>7.36</v>
       </c>
+      <c r="U9" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="V9" s="4">
+        <v>13.8</v>
+      </c>
+      <c r="W9" s="4">
+        <v>1.33E-3</v>
+      </c>
+      <c r="X9" s="4">
+        <v>9.5399999999999999E-3</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>0.82</v>
+      </c>
+      <c r="AA9" s="4">
+        <v>1.79</v>
+      </c>
       <c r="BH9" s="7"/>
       <c r="BM9" s="7"/>
       <c r="BQ9" s="7"/>
@@ -1267,6 +1897,27 @@
       <c r="T10" s="4">
         <v>5.08</v>
       </c>
+      <c r="U10" s="4">
+        <v>2.68</v>
+      </c>
+      <c r="V10" s="4">
+        <v>8.91</v>
+      </c>
+      <c r="W10" s="4">
+        <v>9.3299999999999998E-3</v>
+      </c>
+      <c r="X10" s="4">
+        <v>3.8800000000000001E-2</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="Z10" s="4">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="AA10" s="4">
+        <v>1.69</v>
+      </c>
       <c r="BH10" s="7"/>
       <c r="BM10" s="7"/>
       <c r="BQ10" s="7"/>
@@ -1281,11 +1932,17 @@
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="Z11" s="4">
+        <v>30.9</v>
+      </c>
     </row>
     <row r="12" spans="1:97">
       <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="Z12" s="4">
+        <v>0.43</v>
+      </c>
     </row>
     <row r="17" spans="1:92">
       <c r="A17" s="2" t="s">
@@ -1309,6 +1966,12 @@
       <c r="N17" s="4">
         <v>20</v>
       </c>
+      <c r="W17" s="4">
+        <v>25</v>
+      </c>
+      <c r="Y17" s="4">
+        <v>22</v>
+      </c>
       <c r="CI17"/>
       <c r="CM17" s="4"/>
     </row>
@@ -1337,6 +2000,9 @@
       <c r="O18" s="4">
         <v>66</v>
       </c>
+      <c r="Y18" s="4">
+        <v>70</v>
+      </c>
       <c r="CM18" s="4"/>
     </row>
     <row r="19" spans="1:92">
@@ -1370,6 +2036,9 @@
       <c r="U19" s="4">
         <v>4</v>
       </c>
+      <c r="Y19" s="4">
+        <v>3</v>
+      </c>
       <c r="CM19" s="4"/>
       <c r="CN19" s="4"/>
     </row>
@@ -1420,7 +2089,7 @@
         <v>12</v>
       </c>
       <c r="C22">
-        <v>0.28499999999999998</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="D22" s="6">
         <v>1.1200000000000001</v>
@@ -1479,6 +2148,12 @@
       <c r="U26" s="4">
         <v>7.2</v>
       </c>
+      <c r="W26" s="4">
+        <v>9</v>
+      </c>
+      <c r="Y26" s="4">
+        <v>10</v>
+      </c>
       <c r="CM26" s="4"/>
     </row>
     <row r="27" spans="1:92">
@@ -1497,6 +2172,12 @@
       <c r="U27" s="4">
         <v>3.3</v>
       </c>
+      <c r="W27" s="4">
+        <v>4.125</v>
+      </c>
+      <c r="Y27" s="4">
+        <v>4.58</v>
+      </c>
       <c r="CM27" s="4"/>
     </row>
     <row r="28" spans="1:92">
@@ -1512,6 +2193,15 @@
       <c r="M28" s="4">
         <v>0.18</v>
       </c>
+      <c r="W28" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="Y28" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="AB28" s="4">
+        <v>0.18</v>
+      </c>
       <c r="CM28" s="4"/>
     </row>
     <row r="29" spans="1:92">
@@ -1527,6 +2217,15 @@
       <c r="M29" s="4">
         <v>0.89999999999999991</v>
       </c>
+      <c r="W29" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="Y29" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="AB29" s="4">
+        <v>0.9</v>
+      </c>
       <c r="CM29" s="4"/>
     </row>
     <row r="30" spans="1:92">
@@ -1539,6 +2238,10 @@
       <c r="D30" s="6">
         <v>1.6</v>
       </c>
+      <c r="Y30" s="4">
+        <f>D30*0.85</f>
+        <v>1.36</v>
+      </c>
       <c r="CM30" s="4"/>
     </row>
     <row r="31" spans="1:92">
@@ -1551,6 +2254,10 @@
       <c r="D31" s="6">
         <v>6</v>
       </c>
+      <c r="Y31" s="4">
+        <f>D31*0.85</f>
+        <v>5.0999999999999996</v>
+      </c>
       <c r="CM31" s="4"/>
     </row>
     <row r="32" spans="1:92">
@@ -1590,6 +2297,9 @@
       <c r="R34" s="4">
         <v>6.8000000000000007</v>
       </c>
+      <c r="W34" s="4">
+        <v>6.4</v>
+      </c>
       <c r="CM34" s="4"/>
     </row>
     <row r="35" spans="1:91">
@@ -1608,6 +2318,12 @@
       <c r="U35" s="4">
         <v>6</v>
       </c>
+      <c r="W35" s="4">
+        <v>8</v>
+      </c>
+      <c r="Y35" s="4">
+        <v>7</v>
+      </c>
       <c r="CM35" s="4"/>
     </row>
     <row r="36" spans="1:91">
@@ -1626,6 +2342,12 @@
       <c r="U36" s="4">
         <v>1.6</v>
       </c>
+      <c r="W36" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="AB36" s="4">
+        <v>1.4</v>
+      </c>
       <c r="CM36" s="4"/>
     </row>
     <row r="37" spans="1:91">
@@ -1640,6 +2362,12 @@
       </c>
       <c r="R37" s="4">
         <v>0.44999999999999996</v>
+      </c>
+      <c r="W37" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="Y37" s="4">
+        <v>0.7</v>
       </c>
       <c r="CM37" s="4"/>
     </row>

</xml_diff>

<commit_message>
Refit for a second set of synaptic parameters; change input to 9 assemblies instead of 10; update results from the second set of parameters
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="72">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -294,6 +294,14 @@
   </si>
   <si>
     <t>baseline_13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -683,13 +691,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -700,7 +708,7 @@
     <col min="4" max="4" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:19">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -708,8 +716,50 @@
       <c r="E1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -717,7 +767,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:19">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -727,68 +777,462 @@
       <c r="C3" s="7">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3">
+        <v>2.25</v>
+      </c>
+      <c r="F3">
+        <v>2.16</v>
+      </c>
+      <c r="G3">
+        <v>2.42</v>
+      </c>
+      <c r="H3">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="I3">
+        <v>1.68</v>
+      </c>
+      <c r="J3">
+        <v>2.64</v>
+      </c>
+      <c r="K3">
+        <v>1.67</v>
+      </c>
+      <c r="L3">
+        <v>1.82</v>
+      </c>
+      <c r="M3">
+        <v>1.81</v>
+      </c>
+      <c r="N3">
+        <v>1.26</v>
+      </c>
+      <c r="O3">
+        <v>1.55</v>
+      </c>
+      <c r="P3">
+        <v>1.51</v>
+      </c>
+      <c r="Q3">
+        <v>1.93</v>
+      </c>
+      <c r="R3">
+        <v>2.1</v>
+      </c>
+      <c r="S3">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="7">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4">
+        <v>1.47</v>
+      </c>
+      <c r="F4">
+        <v>1.08</v>
+      </c>
+      <c r="G4">
+        <v>1.01</v>
+      </c>
+      <c r="H4">
+        <v>1.08</v>
+      </c>
+      <c r="I4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J4">
+        <v>1.34</v>
+      </c>
+      <c r="K4">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L4">
+        <v>1.04</v>
+      </c>
+      <c r="M4">
+        <v>1.03</v>
+      </c>
+      <c r="N4">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="O4">
+        <v>0.995</v>
+      </c>
+      <c r="P4">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="Q4">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="R4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S4">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="7">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5">
+        <v>6.35</v>
+      </c>
+      <c r="F5">
+        <v>1.04</v>
+      </c>
+      <c r="G5">
+        <v>1.85</v>
+      </c>
+      <c r="H5">
+        <v>1.45</v>
+      </c>
+      <c r="I5">
+        <v>1.91</v>
+      </c>
+      <c r="J5">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="K5">
+        <v>1.44</v>
+      </c>
+      <c r="L5">
+        <v>2.5</v>
+      </c>
+      <c r="M5">
+        <v>2.73</v>
+      </c>
+      <c r="N5">
+        <v>1.49</v>
+      </c>
+      <c r="O5">
+        <v>1.29</v>
+      </c>
+      <c r="P5">
+        <v>2.57</v>
+      </c>
+      <c r="Q5">
+        <v>1.34</v>
+      </c>
+      <c r="R5">
+        <v>2.39</v>
+      </c>
+      <c r="S5">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="C6" s="7">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="E6">
+        <v>2.69</v>
+      </c>
+      <c r="F6">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="G6">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H6">
+        <v>1.03</v>
+      </c>
+      <c r="I6">
+        <v>1.26</v>
+      </c>
+      <c r="J6">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="K6">
+        <v>1.08</v>
+      </c>
+      <c r="L6">
+        <v>1.26</v>
+      </c>
+      <c r="M6">
+        <v>1.31</v>
+      </c>
+      <c r="N6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O6">
+        <v>1.02</v>
+      </c>
+      <c r="P6">
+        <v>1.31</v>
+      </c>
+      <c r="Q6">
+        <v>1.04</v>
+      </c>
+      <c r="R6">
+        <v>1.23</v>
+      </c>
+      <c r="S6">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="7">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="E7">
+        <v>0.436</v>
+      </c>
+      <c r="F7">
+        <v>6.07</v>
+      </c>
+      <c r="G7">
+        <v>3.91</v>
+      </c>
+      <c r="H7">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="I7">
+        <v>3.61</v>
+      </c>
+      <c r="J7">
+        <v>4.13</v>
+      </c>
+      <c r="K7">
+        <v>3.92</v>
+      </c>
+      <c r="L7">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="M7">
+        <v>3.74</v>
+      </c>
+      <c r="N7">
+        <v>3.45</v>
+      </c>
+      <c r="O7">
+        <v>3.84</v>
+      </c>
+      <c r="P7">
+        <v>3.36</v>
+      </c>
+      <c r="Q7">
+        <v>4.03</v>
+      </c>
+      <c r="R7">
+        <v>4.03</v>
+      </c>
+      <c r="S7">
+        <v>3.57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="C8" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8">
+        <v>1.48</v>
+      </c>
+      <c r="F8">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="G8">
+        <v>4.72</v>
+      </c>
+      <c r="H8">
+        <v>5.98</v>
+      </c>
+      <c r="I8">
+        <v>5.36</v>
+      </c>
+      <c r="J8">
+        <v>5.74</v>
+      </c>
+      <c r="K8">
+        <v>5.66</v>
+      </c>
+      <c r="L8">
+        <v>5.72</v>
+      </c>
+      <c r="M8">
+        <v>5.58</v>
+      </c>
+      <c r="N8">
+        <v>5.23</v>
+      </c>
+      <c r="O8">
+        <v>5.58</v>
+      </c>
+      <c r="P8">
+        <v>5.22</v>
+      </c>
+      <c r="Q8">
+        <v>5.66</v>
+      </c>
+      <c r="R8">
+        <v>5.58</v>
+      </c>
+      <c r="S8">
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="7">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9">
+        <v>29.4</v>
+      </c>
+      <c r="F9">
+        <v>6.6199999999999995E-2</v>
+      </c>
+      <c r="G9">
+        <v>1.84</v>
+      </c>
+      <c r="H9">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="I9">
+        <v>1.2</v>
+      </c>
+      <c r="J9">
+        <v>0.115</v>
+      </c>
+      <c r="K9">
+        <v>0.377</v>
+      </c>
+      <c r="L9">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="M9">
+        <v>2.85</v>
+      </c>
+      <c r="N9">
+        <v>3.17</v>
+      </c>
+      <c r="O9">
+        <v>2.59</v>
+      </c>
+      <c r="P9">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="Q9">
+        <v>1.41</v>
+      </c>
+      <c r="R9">
+        <v>5.68</v>
+      </c>
+      <c r="S9">
+        <v>6.81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="C10" s="7">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10">
+        <v>10.7</v>
+      </c>
+      <c r="F10">
+        <v>0.128</v>
+      </c>
+      <c r="G10">
+        <v>1.52</v>
+      </c>
+      <c r="H10">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="I10">
+        <v>1.23</v>
+      </c>
+      <c r="J10">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="K10">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="L10">
+        <v>1.9</v>
+      </c>
+      <c r="M10">
+        <v>2.17</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <v>1.76</v>
+      </c>
+      <c r="P10">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="Q10">
+        <v>1.24</v>
+      </c>
+      <c r="R10">
+        <v>3.24</v>
+      </c>
+      <c r="S10">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <v>34</v>
+      </c>
+      <c r="G11">
+        <v>31.9</v>
+      </c>
+      <c r="L11">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="R11">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F12">
+        <v>1.9</v>
+      </c>
+      <c r="G12">
+        <v>1.2</v>
+      </c>
+      <c r="L12">
+        <v>0.43</v>
+      </c>
+      <c r="R12">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="F13">
+        <v>66.900000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -799,8 +1243,32 @@
         <v>22</v>
       </c>
       <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17">
+        <v>20</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <v>12</v>
+      </c>
+      <c r="J17">
+        <v>14</v>
+      </c>
+      <c r="K17">
+        <v>11</v>
+      </c>
+      <c r="N17">
+        <v>12</v>
+      </c>
+      <c r="O17">
+        <v>13</v>
+      </c>
+      <c r="Q17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
@@ -808,8 +1276,26 @@
         <v>70</v>
       </c>
       <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="H18">
+        <v>60</v>
+      </c>
+      <c r="I18">
+        <v>36</v>
+      </c>
+      <c r="J18">
+        <v>24</v>
+      </c>
+      <c r="K18">
+        <v>32</v>
+      </c>
+      <c r="O18">
+        <v>31</v>
+      </c>
+      <c r="Q18">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
@@ -817,8 +1303,29 @@
         <v>3</v>
       </c>
       <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>3.6</v>
+      </c>
+      <c r="J19">
+        <v>3.8</v>
+      </c>
+      <c r="K19">
+        <v>3.8</v>
+      </c>
+      <c r="N19">
+        <v>3.5</v>
+      </c>
+      <c r="O19">
+        <v>3.7</v>
+      </c>
+      <c r="Q19">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
@@ -826,12 +1333,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:17">
       <c r="C21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:17">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -845,7 +1352,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:17">
       <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
@@ -856,7 +1363,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:17">
       <c r="B24" s="2" t="s">
         <v>15</v>
       </c>
@@ -867,7 +1374,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:17">
       <c r="B25" s="2" t="s">
         <v>14</v>
       </c>
@@ -878,7 +1385,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:17">
       <c r="B26" s="2" t="s">
         <v>16</v>
       </c>
@@ -888,8 +1395,26 @@
       <c r="D26" s="6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26">
+        <v>6.95</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="N26">
+        <v>4.5</v>
+      </c>
+      <c r="O26">
+        <v>4.25</v>
+      </c>
+      <c r="Q26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="B27" s="2" t="s">
         <v>17</v>
       </c>
@@ -899,8 +1424,26 @@
       <c r="D27" s="6">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <v>4.58</v>
+      </c>
+      <c r="G27">
+        <v>3.3</v>
+      </c>
+      <c r="H27">
+        <v>2.64</v>
+      </c>
+      <c r="N27">
+        <v>2.97</v>
+      </c>
+      <c r="O27">
+        <v>2.8</v>
+      </c>
+      <c r="Q27">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
@@ -910,8 +1453,14 @@
       <c r="D28" s="6">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="N28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q28">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="B29" s="2" t="s">
         <v>19</v>
       </c>
@@ -921,8 +1470,14 @@
       <c r="D29" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="N29">
+        <v>0.7</v>
+      </c>
+      <c r="Q29">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="B30" s="2" t="s">
         <v>20</v>
       </c>
@@ -932,8 +1487,14 @@
       <c r="D30" s="6">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30">
+        <v>12.1</v>
+      </c>
+      <c r="I30" s="6">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="B31" s="2" t="s">
         <v>21</v>
       </c>
@@ -943,8 +1504,14 @@
       <c r="D31" s="6">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31">
+        <v>43.5</v>
+      </c>
+      <c r="I31" s="6">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="B32" s="2" t="s">
         <v>22</v>
       </c>
@@ -954,8 +1521,17 @@
       <c r="D32" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="I32" s="6">
+        <v>2</v>
+      </c>
+      <c r="N32">
+        <v>1.5</v>
+      </c>
+      <c r="Q32">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
@@ -965,8 +1541,17 @@
       <c r="D33" s="6">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="I33" s="6">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="B34" s="2" t="s">
         <v>23</v>
       </c>
@@ -976,8 +1561,14 @@
       <c r="D34" s="6">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="F34">
+        <v>6.4</v>
+      </c>
+      <c r="N34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="B35" s="2" t="s">
         <v>25</v>
       </c>
@@ -987,8 +1578,20 @@
       <c r="D35" s="6">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="F35">
+        <v>7</v>
+      </c>
+      <c r="G35">
+        <v>6</v>
+      </c>
+      <c r="O35">
+        <v>7</v>
+      </c>
+      <c r="Q35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="B36" s="2" t="s">
         <v>26</v>
       </c>
@@ -998,8 +1601,17 @@
       <c r="D36" s="6">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="F36">
+        <v>1.4</v>
+      </c>
+      <c r="N36">
+        <v>1.2</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="B37" s="2" t="s">
         <v>24</v>
       </c>
@@ -1009,13 +1621,16 @@
       <c r="D37" s="6">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="N37">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="C38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:17">
       <c r="A39" s="2" t="s">
         <v>40</v>
       </c>
@@ -1026,7 +1641,7 @@
         <v>1.7000000000000001E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:17">
       <c r="B40" s="2" t="s">
         <v>24</v>
       </c>
@@ -1034,7 +1649,7 @@
         <v>1.9000000000000001E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:17">
       <c r="A42" s="2" t="s">
         <v>33</v>
       </c>
@@ -1042,22 +1657,22 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:17">
       <c r="B43" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:17">
       <c r="B44" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:17">
       <c r="B45" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:17">
       <c r="A46" s="2" t="s">
         <v>33</v>
       </c>
@@ -1065,12 +1680,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:17">
       <c r="B47" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:17">
       <c r="B48" s="2" t="s">
         <v>18</v>
       </c>
@@ -1119,10 +1734,10 @@
   <dimension ref="A1:CV58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="W21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y17" sqref="Y17:Y19"/>
+      <selection pane="bottomRight" activeCell="Y27" sqref="Y26:Y27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
Correct error in exp2syn_stp that causes inconsistent stp variables for multiple sources; update a new set of synaptic parameters
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -7,15 +7,17 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
-    <sheet name="set 2" sheetId="5" r:id="rId1"/>
-    <sheet name="set 1" sheetId="3" r:id="rId2"/>
+    <sheet name="new set" sheetId="7" r:id="rId1"/>
+    <sheet name="init as M1" sheetId="6" r:id="rId2"/>
+    <sheet name="set 2" sheetId="5" r:id="rId3"/>
+    <sheet name="set 1" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="106">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -302,6 +304,142 @@
   </si>
   <si>
     <t>long_6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_test_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_test_17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_test_18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_test_20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2, tau2=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.8, tau2=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_test_21</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -691,83 +829,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
+      <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="13.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
-    <col min="4" max="4" width="9" style="6"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:5">
+      <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
+      <c r="D1" s="6"/>
       <c r="E1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -777,462 +871,133 @@
       <c r="C3" s="7">
         <v>1.9</v>
       </c>
+      <c r="D3" s="6"/>
       <c r="E3">
-        <v>2.25</v>
-      </c>
-      <c r="F3">
-        <v>2.16</v>
-      </c>
-      <c r="G3">
-        <v>2.42</v>
-      </c>
-      <c r="H3">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="I3">
-        <v>1.68</v>
-      </c>
-      <c r="J3">
-        <v>2.64</v>
-      </c>
-      <c r="K3">
-        <v>1.67</v>
-      </c>
-      <c r="L3">
-        <v>1.82</v>
-      </c>
-      <c r="M3">
-        <v>1.81</v>
-      </c>
-      <c r="N3">
-        <v>1.26</v>
-      </c>
-      <c r="O3">
-        <v>1.55</v>
-      </c>
-      <c r="P3">
-        <v>1.51</v>
-      </c>
-      <c r="Q3">
-        <v>1.93</v>
-      </c>
-      <c r="R3">
-        <v>2.1</v>
-      </c>
-      <c r="S3">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="7">
-        <v>1.3</v>
-      </c>
+        <v>1.4</v>
+      </c>
+      <c r="D4" s="6"/>
       <c r="E4">
-        <v>1.47</v>
-      </c>
-      <c r="F4">
-        <v>1.08</v>
-      </c>
-      <c r="G4">
-        <v>1.01</v>
-      </c>
-      <c r="H4">
-        <v>1.08</v>
-      </c>
-      <c r="I4">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="J4">
         <v>1.34</v>
       </c>
-      <c r="K4">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L4">
-        <v>1.04</v>
-      </c>
-      <c r="M4">
-        <v>1.03</v>
-      </c>
-      <c r="N4">
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="O4">
-        <v>0.995</v>
-      </c>
-      <c r="P4">
-        <v>0.96299999999999997</v>
-      </c>
-      <c r="Q4">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="R4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="S4">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="7">
-        <v>1.35</v>
-      </c>
+        <v>1.3</v>
+      </c>
+      <c r="D5" s="6"/>
       <c r="E5">
-        <v>6.35</v>
-      </c>
-      <c r="F5">
-        <v>1.04</v>
-      </c>
-      <c r="G5">
-        <v>1.85</v>
-      </c>
-      <c r="H5">
-        <v>1.45</v>
-      </c>
-      <c r="I5">
-        <v>1.91</v>
-      </c>
-      <c r="J5">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="K5">
         <v>1.44</v>
       </c>
-      <c r="L5">
-        <v>2.5</v>
-      </c>
-      <c r="M5">
-        <v>2.73</v>
-      </c>
-      <c r="N5">
-        <v>1.49</v>
-      </c>
-      <c r="O5">
-        <v>1.29</v>
-      </c>
-      <c r="P5">
-        <v>2.57</v>
-      </c>
-      <c r="Q5">
-        <v>1.34</v>
-      </c>
-      <c r="R5">
-        <v>2.39</v>
-      </c>
-      <c r="S5">
-        <v>2.69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="7">
-        <v>1.2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D6" s="6"/>
       <c r="E6">
-        <v>2.69</v>
-      </c>
-      <c r="F6">
-        <v>0.79400000000000004</v>
-      </c>
-      <c r="G6">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="H6">
-        <v>1.03</v>
-      </c>
-      <c r="I6">
-        <v>1.26</v>
-      </c>
-      <c r="J6">
-        <v>0.67700000000000005</v>
-      </c>
-      <c r="K6">
-        <v>1.08</v>
-      </c>
-      <c r="L6">
-        <v>1.26</v>
-      </c>
-      <c r="M6">
-        <v>1.31</v>
-      </c>
-      <c r="N6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="O6">
-        <v>1.02</v>
-      </c>
-      <c r="P6">
-        <v>1.31</v>
-      </c>
-      <c r="Q6">
-        <v>1.04</v>
-      </c>
-      <c r="R6">
-        <v>1.23</v>
-      </c>
-      <c r="S6">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="7">
-        <v>4.0999999999999996</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D7" s="6"/>
       <c r="E7">
-        <v>0.436</v>
-      </c>
-      <c r="F7">
-        <v>6.07</v>
-      </c>
-      <c r="G7">
-        <v>3.91</v>
-      </c>
-      <c r="H7">
-        <v>4.5199999999999996</v>
-      </c>
-      <c r="I7">
-        <v>3.61</v>
-      </c>
-      <c r="J7">
-        <v>4.13</v>
-      </c>
-      <c r="K7">
-        <v>3.92</v>
-      </c>
-      <c r="L7">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="M7">
-        <v>3.74</v>
-      </c>
-      <c r="N7">
-        <v>3.45</v>
-      </c>
-      <c r="O7">
-        <v>3.84</v>
-      </c>
-      <c r="P7">
-        <v>3.36</v>
-      </c>
-      <c r="Q7">
-        <v>4.03</v>
-      </c>
-      <c r="R7">
-        <v>4.03</v>
-      </c>
-      <c r="S7">
-        <v>3.57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19">
+        <v>0.99399999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="7">
         <v>6</v>
       </c>
+      <c r="D8" s="6"/>
       <c r="E8">
-        <v>1.48</v>
-      </c>
-      <c r="F8">
-        <v>4.8099999999999996</v>
-      </c>
-      <c r="G8">
-        <v>4.72</v>
-      </c>
-      <c r="H8">
-        <v>5.98</v>
-      </c>
-      <c r="I8">
-        <v>5.36</v>
-      </c>
-      <c r="J8">
-        <v>5.74</v>
-      </c>
-      <c r="K8">
-        <v>5.66</v>
-      </c>
-      <c r="L8">
-        <v>5.72</v>
-      </c>
-      <c r="M8">
-        <v>5.58</v>
-      </c>
-      <c r="N8">
-        <v>5.23</v>
-      </c>
-      <c r="O8">
-        <v>5.58</v>
-      </c>
-      <c r="P8">
-        <v>5.22</v>
-      </c>
-      <c r="Q8">
-        <v>5.66</v>
-      </c>
-      <c r="R8">
-        <v>5.58</v>
-      </c>
-      <c r="S8">
-        <v>5.44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="7">
-        <v>0.2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D9" s="6"/>
       <c r="E9">
-        <v>29.4</v>
-      </c>
-      <c r="F9">
-        <v>6.6199999999999995E-2</v>
-      </c>
-      <c r="G9">
-        <v>1.84</v>
-      </c>
-      <c r="H9">
-        <v>0.72599999999999998</v>
-      </c>
-      <c r="I9">
-        <v>1.2</v>
-      </c>
-      <c r="J9">
-        <v>0.115</v>
-      </c>
-      <c r="K9">
-        <v>0.377</v>
-      </c>
-      <c r="L9">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="M9">
-        <v>2.85</v>
-      </c>
-      <c r="N9">
-        <v>3.17</v>
-      </c>
-      <c r="O9">
-        <v>2.59</v>
-      </c>
-      <c r="P9">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="Q9">
-        <v>1.41</v>
-      </c>
-      <c r="R9">
-        <v>5.68</v>
-      </c>
-      <c r="S9">
-        <v>6.81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19">
+        <v>4.76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="7">
-        <v>0.8</v>
-      </c>
+        <v>2.5</v>
+      </c>
+      <c r="D10" s="6"/>
       <c r="E10">
-        <v>10.7</v>
-      </c>
-      <c r="F10">
-        <v>0.128</v>
-      </c>
-      <c r="G10">
-        <v>1.52</v>
-      </c>
-      <c r="H10">
-        <v>0.79100000000000004</v>
-      </c>
-      <c r="I10">
-        <v>1.23</v>
-      </c>
-      <c r="J10">
-        <v>0.21099999999999999</v>
-      </c>
-      <c r="K10">
-        <v>0.51100000000000001</v>
-      </c>
-      <c r="L10">
-        <v>1.9</v>
-      </c>
-      <c r="M10">
-        <v>2.17</v>
-      </c>
-      <c r="N10">
-        <v>2</v>
-      </c>
-      <c r="O10">
-        <v>1.76</v>
-      </c>
-      <c r="P10">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="Q10">
-        <v>1.24</v>
-      </c>
-      <c r="R10">
-        <v>3.24</v>
-      </c>
-      <c r="S10">
-        <v>3.66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19">
+        <v>4.8499999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F11">
-        <v>34</v>
-      </c>
-      <c r="G11">
-        <v>31.9</v>
-      </c>
-      <c r="L11">
-        <v>35.700000000000003</v>
-      </c>
-      <c r="R11">
-        <v>35.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F12">
-        <v>1.9</v>
-      </c>
-      <c r="G12">
-        <v>1.2</v>
-      </c>
-      <c r="L12">
-        <v>0.43</v>
-      </c>
-      <c r="R12">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="F13">
-        <v>66.900000000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1242,103 +1007,64 @@
       <c r="D17" s="6">
         <v>22</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="G17">
-        <v>20</v>
-      </c>
-      <c r="H17">
-        <v>16</v>
-      </c>
-      <c r="I17">
-        <v>12</v>
-      </c>
-      <c r="J17">
+      <c r="E17">
         <v>14</v>
       </c>
-      <c r="K17">
+      <c r="F17">
         <v>11</v>
       </c>
-      <c r="N17">
-        <v>12</v>
-      </c>
-      <c r="O17">
-        <v>13</v>
-      </c>
-      <c r="Q17">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="6">
         <v>70</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="H18">
-        <v>60</v>
-      </c>
-      <c r="I18">
-        <v>36</v>
-      </c>
-      <c r="J18">
-        <v>24</v>
-      </c>
-      <c r="K18">
-        <v>32</v>
-      </c>
-      <c r="O18">
-        <v>31</v>
-      </c>
-      <c r="Q18">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="E18">
+        <v>33</v>
+      </c>
+      <c r="F18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="6">
         <v>3</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="H19">
+      <c r="E19" s="4">
+        <v>3</v>
+      </c>
+      <c r="F19">
         <v>4</v>
       </c>
-      <c r="I19">
-        <v>3.6</v>
-      </c>
-      <c r="J19">
-        <v>3.8</v>
-      </c>
-      <c r="K19">
-        <v>3.8</v>
-      </c>
-      <c r="N19">
-        <v>3.5</v>
-      </c>
-      <c r="O19">
-        <v>3.7</v>
-      </c>
-      <c r="Q19">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="6">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="E20" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
       <c r="C21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -1346,212 +1072,176 @@
         <v>12</v>
       </c>
       <c r="C22">
-        <v>0.28499999999999998</v>
+        <v>0.25</v>
       </c>
       <c r="D22" s="6">
-        <v>1.1200000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
+        <v>0.78</v>
+      </c>
+      <c r="F22">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C23">
-        <v>0.13800000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="D23" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
+        <v>0.42</v>
+      </c>
+      <c r="F23">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C24">
-        <v>0.152</v>
+        <v>0.156</v>
       </c>
       <c r="D24" s="6">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
+        <v>0.52</v>
+      </c>
+      <c r="F24">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C25">
-        <v>0.22700000000000001</v>
+        <v>0.224</v>
       </c>
       <c r="D25" s="6">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
+        <v>1.6</v>
+      </c>
+      <c r="F25">
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C26">
-        <v>0.57499999999999996</v>
+        <v>0.58899999999999997</v>
       </c>
       <c r="D26" s="6">
-        <v>2.5</v>
+        <v>1.9</v>
       </c>
       <c r="F26">
-        <v>6.95</v>
-      </c>
-      <c r="G26">
-        <v>5</v>
-      </c>
-      <c r="H26">
-        <v>4</v>
-      </c>
-      <c r="N26">
-        <v>4.5</v>
-      </c>
-      <c r="O26">
-        <v>4.25</v>
-      </c>
-      <c r="Q26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C27">
-        <v>0.39600000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="D27" s="6">
-        <v>1.65</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <v>4.58</v>
-      </c>
-      <c r="G27">
-        <v>3.3</v>
-      </c>
-      <c r="H27">
-        <v>2.64</v>
-      </c>
-      <c r="N27">
-        <v>2.97</v>
-      </c>
-      <c r="O27">
-        <v>2.8</v>
-      </c>
-      <c r="Q27">
-        <v>2.64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C28">
-        <v>3.3000000000000002E-2</v>
+        <v>3.15E-2</v>
       </c>
       <c r="D28" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="N28">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="Q28">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C29">
-        <v>0.11</v>
+        <v>0.106</v>
       </c>
       <c r="D29" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="N29">
-        <v>0.7</v>
-      </c>
-      <c r="Q29">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C30">
-        <v>1.79</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="D30" s="6">
-        <v>6.4</v>
+        <v>3.9</v>
       </c>
       <c r="F30">
-        <v>12.1</v>
-      </c>
-      <c r="I30" s="6">
-        <v>11.2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C31">
-        <v>6.67</v>
+        <v>6.4</v>
       </c>
       <c r="D31" s="6">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F31">
-        <v>43.5</v>
-      </c>
-      <c r="I31" s="6">
-        <v>18.600000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C32">
-        <v>0.68</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="D32" s="6">
-        <v>2</v>
-      </c>
-      <c r="I32" s="6">
-        <v>2</v>
-      </c>
-      <c r="N32">
-        <v>1.5</v>
-      </c>
-      <c r="Q32">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
+        <v>1.75</v>
+      </c>
+      <c r="F32">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C33">
-        <v>0.88800000000000001</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="D33" s="6">
-        <v>2.4</v>
-      </c>
-      <c r="I33" s="6">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="N33">
+        <v>2</v>
+      </c>
+      <c r="F33">
         <v>1</v>
       </c>
-      <c r="Q33">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
         <v>23</v>
       </c>
@@ -1559,78 +1249,63 @@
         <v>1.87</v>
       </c>
       <c r="D34" s="6">
-        <v>8.5</v>
+        <v>5.5</v>
       </c>
       <c r="F34">
-        <v>6.4</v>
-      </c>
-      <c r="N34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C35">
-        <v>1.56</v>
+        <v>1.57</v>
       </c>
       <c r="D35" s="6">
-        <v>6</v>
+        <v>3.65</v>
       </c>
       <c r="F35">
-        <v>7</v>
-      </c>
-      <c r="G35">
-        <v>6</v>
-      </c>
-      <c r="O35">
-        <v>7</v>
-      </c>
-      <c r="Q35">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C36">
-        <v>0.76800000000000002</v>
+        <v>0.52800000000000002</v>
       </c>
       <c r="D36" s="6">
         <v>2.4</v>
       </c>
       <c r="F36">
-        <v>1.4</v>
-      </c>
-      <c r="N36">
         <v>1.2</v>
       </c>
-      <c r="Q36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17">
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C37">
-        <v>0.432</v>
+        <v>0.4</v>
       </c>
       <c r="D37" s="6">
-        <v>0.92</v>
-      </c>
-      <c r="N37">
         <v>0.8</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:6">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
       <c r="C38" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="39" spans="1:17">
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
         <v>40</v>
       </c>
@@ -1641,7 +1316,8 @@
         <v>1.7000000000000001E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:6">
+      <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
         <v>24</v>
       </c>
@@ -1649,79 +1325,127 @@
         <v>1.9000000000000001E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="41" spans="1:6">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="43" spans="1:17">
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="44" spans="1:17">
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:17">
+      <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="46" spans="1:17">
+      <c r="D45" s="6"/>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="47" spans="1:17">
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="48" spans="1:17">
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="D48" s="6"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="D49" s="6"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="D50" s="6"/>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="D51" s="6"/>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="B52" s="2"/>
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="B53" s="2"/>
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B58" s="2"/>
+      <c r="D58" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1731,20 +1455,2998 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CV58"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="W21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y27" sqref="Y26:Y27"/>
+      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="6"/>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="7">
+        <v>6.8</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="7">
+        <v>5.9</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="6">
+        <v>22</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6">
+        <v>70</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="6">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>0.25</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>0.156</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>0.224</v>
+      </c>
+      <c r="D25" s="6">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="D26" s="6">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>0.4</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28">
+        <v>3.15E-2</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29">
+        <v>0.106</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="D30" s="6">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>6.4</v>
+      </c>
+      <c r="D31" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="D32" s="6">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="D33" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <v>1.87</v>
+      </c>
+      <c r="D34" s="6">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>1.57</v>
+      </c>
+      <c r="D35" s="6">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="D36" s="6">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37">
+        <v>0.4</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1.7000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="6">
+        <v>1.9000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="6"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="6"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="6"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="6"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D49" s="6"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="D50" s="6"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="6"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="D58" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:BB58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="AO15" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34:D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="13.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.125" customWidth="1"/>
+    <col min="1" max="1" width="10" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="9" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:54">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54">
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1.9</v>
+      </c>
+      <c r="E3">
+        <v>2.25</v>
+      </c>
+      <c r="F3">
+        <v>2.16</v>
+      </c>
+      <c r="G3">
+        <v>2.42</v>
+      </c>
+      <c r="H3">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="I3">
+        <v>1.68</v>
+      </c>
+      <c r="J3">
+        <v>2.64</v>
+      </c>
+      <c r="K3">
+        <v>1.67</v>
+      </c>
+      <c r="L3">
+        <v>1.82</v>
+      </c>
+      <c r="M3">
+        <v>1.81</v>
+      </c>
+      <c r="N3">
+        <v>1.26</v>
+      </c>
+      <c r="O3">
+        <v>1.55</v>
+      </c>
+      <c r="P3">
+        <v>1.51</v>
+      </c>
+      <c r="Q3">
+        <v>1.93</v>
+      </c>
+      <c r="R3">
+        <v>2.1</v>
+      </c>
+      <c r="S3">
+        <v>2.1</v>
+      </c>
+      <c r="T3">
+        <v>1.63</v>
+      </c>
+      <c r="U3">
+        <v>1.63</v>
+      </c>
+      <c r="V3">
+        <v>2.1</v>
+      </c>
+      <c r="W3">
+        <v>1.6</v>
+      </c>
+      <c r="X3">
+        <v>1.63</v>
+      </c>
+      <c r="Y3">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="Z3">
+        <v>2.1</v>
+      </c>
+      <c r="AA3">
+        <v>3.22</v>
+      </c>
+      <c r="AB3">
+        <v>1.93</v>
+      </c>
+      <c r="AC3">
+        <v>1.65</v>
+      </c>
+      <c r="AD3">
+        <v>1.6</v>
+      </c>
+      <c r="AE3">
+        <v>1.69</v>
+      </c>
+      <c r="AF3">
+        <v>1.99</v>
+      </c>
+      <c r="AG3">
+        <v>1.58</v>
+      </c>
+      <c r="AH3">
+        <v>1.55</v>
+      </c>
+      <c r="AI3">
+        <v>1.88</v>
+      </c>
+      <c r="AJ3">
+        <v>1.85</v>
+      </c>
+      <c r="AK3">
+        <v>1.47</v>
+      </c>
+      <c r="AL3">
+        <v>1.82</v>
+      </c>
+      <c r="AM3">
+        <v>2.23</v>
+      </c>
+      <c r="AN3">
+        <v>2.06</v>
+      </c>
+      <c r="AO3">
+        <v>1.79</v>
+      </c>
+      <c r="AP3">
+        <v>2.33</v>
+      </c>
+      <c r="AQ3">
+        <v>2.27</v>
+      </c>
+      <c r="AR3">
+        <v>1.86</v>
+      </c>
+      <c r="AS3">
+        <v>1.9</v>
+      </c>
+      <c r="AT3">
+        <v>3.15</v>
+      </c>
+      <c r="AU3">
+        <v>3.08</v>
+      </c>
+      <c r="AV3">
+        <v>2.93</v>
+      </c>
+      <c r="AW3">
+        <v>1.71</v>
+      </c>
+      <c r="AX3">
+        <v>2.75</v>
+      </c>
+      <c r="AY3">
+        <v>2.57</v>
+      </c>
+      <c r="AZ3">
+        <v>1.7</v>
+      </c>
+      <c r="BA3">
+        <v>2.46</v>
+      </c>
+      <c r="BB3">
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="E4">
+        <v>1.47</v>
+      </c>
+      <c r="F4">
+        <v>1.08</v>
+      </c>
+      <c r="G4">
+        <v>1.01</v>
+      </c>
+      <c r="H4">
+        <v>1.08</v>
+      </c>
+      <c r="I4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J4">
+        <v>1.34</v>
+      </c>
+      <c r="K4">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L4">
+        <v>1.04</v>
+      </c>
+      <c r="M4">
+        <v>1.03</v>
+      </c>
+      <c r="N4">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="O4">
+        <v>0.995</v>
+      </c>
+      <c r="P4">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="Q4">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="R4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T4">
+        <v>1.05</v>
+      </c>
+      <c r="U4">
+        <v>1.01</v>
+      </c>
+      <c r="V4">
+        <v>1.18</v>
+      </c>
+      <c r="W4">
+        <v>1.04</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>1.08</v>
+      </c>
+      <c r="Z4">
+        <v>1.21</v>
+      </c>
+      <c r="AA4">
+        <v>1.65</v>
+      </c>
+      <c r="AB4">
+        <v>1.31</v>
+      </c>
+      <c r="AC4">
+        <v>1.17</v>
+      </c>
+      <c r="AD4">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AE4">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="AF4">
+        <v>1.33</v>
+      </c>
+      <c r="AG4">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AH4">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="AI4">
+        <v>1.38</v>
+      </c>
+      <c r="AJ4">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AK4">
+        <v>1.05</v>
+      </c>
+      <c r="AL4">
+        <v>1.36</v>
+      </c>
+      <c r="AM4">
+        <v>1.25</v>
+      </c>
+      <c r="AN4">
+        <v>1.24</v>
+      </c>
+      <c r="AO4">
+        <v>1.31</v>
+      </c>
+      <c r="AP4">
+        <v>1.24</v>
+      </c>
+      <c r="AQ4">
+        <v>1.25</v>
+      </c>
+      <c r="AR4">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="AS4">
+        <v>1.65</v>
+      </c>
+      <c r="AT4">
+        <v>1.71</v>
+      </c>
+      <c r="AU4">
+        <v>1.71</v>
+      </c>
+      <c r="AV4">
+        <v>1.67</v>
+      </c>
+      <c r="AW4">
+        <v>1.59</v>
+      </c>
+      <c r="AX4">
+        <v>1.63</v>
+      </c>
+      <c r="AY4">
+        <v>1.57</v>
+      </c>
+      <c r="AZ4">
+        <v>1.56</v>
+      </c>
+      <c r="BA4">
+        <v>1.49</v>
+      </c>
+      <c r="BB4">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1.35</v>
+      </c>
+      <c r="E5">
+        <v>6.35</v>
+      </c>
+      <c r="F5">
+        <v>1.04</v>
+      </c>
+      <c r="G5">
+        <v>1.85</v>
+      </c>
+      <c r="H5">
+        <v>1.45</v>
+      </c>
+      <c r="I5">
+        <v>1.91</v>
+      </c>
+      <c r="J5">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="K5">
+        <v>1.44</v>
+      </c>
+      <c r="L5">
+        <v>2.5</v>
+      </c>
+      <c r="M5">
+        <v>2.73</v>
+      </c>
+      <c r="N5">
+        <v>1.49</v>
+      </c>
+      <c r="O5">
+        <v>1.29</v>
+      </c>
+      <c r="P5">
+        <v>2.57</v>
+      </c>
+      <c r="Q5">
+        <v>1.34</v>
+      </c>
+      <c r="R5">
+        <v>2.39</v>
+      </c>
+      <c r="S5">
+        <v>2.69</v>
+      </c>
+      <c r="T5">
+        <v>1.35</v>
+      </c>
+      <c r="U5">
+        <v>2.78</v>
+      </c>
+      <c r="V5">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="W5">
+        <v>1.32</v>
+      </c>
+      <c r="X5">
+        <v>2.83</v>
+      </c>
+      <c r="Y5">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="Z5">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="AA5">
+        <v>3.03</v>
+      </c>
+      <c r="AB5">
+        <v>1.33</v>
+      </c>
+      <c r="AC5">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AD5">
+        <v>2.78</v>
+      </c>
+      <c r="AE5">
+        <v>1.27</v>
+      </c>
+      <c r="AF5">
+        <v>1.31</v>
+      </c>
+      <c r="AG5">
+        <v>2.59</v>
+      </c>
+      <c r="AH5">
+        <v>2.78</v>
+      </c>
+      <c r="AI5">
+        <v>1.46</v>
+      </c>
+      <c r="AJ5">
+        <v>2.42</v>
+      </c>
+      <c r="AK5">
+        <v>3.11</v>
+      </c>
+      <c r="AL5">
+        <v>1.39</v>
+      </c>
+      <c r="AM5">
+        <v>2.23</v>
+      </c>
+      <c r="AN5">
+        <v>2.83</v>
+      </c>
+      <c r="AO5">
+        <v>1.25</v>
+      </c>
+      <c r="AP5">
+        <v>1.94</v>
+      </c>
+      <c r="AQ5">
+        <v>2.46</v>
+      </c>
+      <c r="AR5">
+        <v>2.91</v>
+      </c>
+      <c r="AS5">
+        <v>1.33</v>
+      </c>
+      <c r="AT5">
+        <v>2.16</v>
+      </c>
+      <c r="AU5">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="AV5">
+        <v>2.56</v>
+      </c>
+      <c r="AW5">
+        <v>1.47</v>
+      </c>
+      <c r="AX5">
+        <v>2.44</v>
+      </c>
+      <c r="AY5">
+        <v>2.86</v>
+      </c>
+      <c r="AZ5">
+        <v>1.37</v>
+      </c>
+      <c r="BA5">
+        <v>2.62</v>
+      </c>
+      <c r="BB5">
+        <v>4.03</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54">
+      <c r="C6" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="E6">
+        <v>2.69</v>
+      </c>
+      <c r="F6">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="G6">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H6">
+        <v>1.03</v>
+      </c>
+      <c r="I6">
+        <v>1.26</v>
+      </c>
+      <c r="J6">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="K6">
+        <v>1.08</v>
+      </c>
+      <c r="L6">
+        <v>1.26</v>
+      </c>
+      <c r="M6">
+        <v>1.31</v>
+      </c>
+      <c r="N6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O6">
+        <v>1.02</v>
+      </c>
+      <c r="P6">
+        <v>1.31</v>
+      </c>
+      <c r="Q6">
+        <v>1.04</v>
+      </c>
+      <c r="R6">
+        <v>1.23</v>
+      </c>
+      <c r="S6">
+        <v>1.3</v>
+      </c>
+      <c r="T6">
+        <v>1.04</v>
+      </c>
+      <c r="U6">
+        <v>1.35</v>
+      </c>
+      <c r="V6">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="W6">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="X6">
+        <v>1.4</v>
+      </c>
+      <c r="Y6">
+        <v>2.12</v>
+      </c>
+      <c r="Z6">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="AA6">
+        <v>1.58</v>
+      </c>
+      <c r="AB6">
+        <v>1.05</v>
+      </c>
+      <c r="AC6">
+        <v>1.26</v>
+      </c>
+      <c r="AD6">
+        <v>1.32</v>
+      </c>
+      <c r="AE6">
+        <v>1.03</v>
+      </c>
+      <c r="AF6">
+        <v>1.05</v>
+      </c>
+      <c r="AG6">
+        <v>1.28</v>
+      </c>
+      <c r="AH6">
+        <v>1.33</v>
+      </c>
+      <c r="AI6">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="AJ6">
+        <v>1.21</v>
+      </c>
+      <c r="AK6">
+        <v>1.37</v>
+      </c>
+      <c r="AL6">
+        <v>1.07</v>
+      </c>
+      <c r="AM6">
+        <v>1.18</v>
+      </c>
+      <c r="AN6">
+        <v>1.31</v>
+      </c>
+      <c r="AO6">
+        <v>1.01</v>
+      </c>
+      <c r="AP6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AQ6">
+        <v>1.21</v>
+      </c>
+      <c r="AR6">
+        <v>1.32</v>
+      </c>
+      <c r="AS6">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="AT6">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AU6">
+        <v>1.22</v>
+      </c>
+      <c r="AV6">
+        <v>1.25</v>
+      </c>
+      <c r="AW6">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AX6">
+        <v>1.23</v>
+      </c>
+      <c r="AY6">
+        <v>1.33</v>
+      </c>
+      <c r="AZ6">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="BA6">
+        <v>1.26</v>
+      </c>
+      <c r="BB6">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54">
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E7">
+        <v>0.436</v>
+      </c>
+      <c r="F7">
+        <v>6.07</v>
+      </c>
+      <c r="G7">
+        <v>3.91</v>
+      </c>
+      <c r="H7">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="I7">
+        <v>3.61</v>
+      </c>
+      <c r="J7">
+        <v>4.13</v>
+      </c>
+      <c r="K7">
+        <v>3.92</v>
+      </c>
+      <c r="L7">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="M7">
+        <v>3.74</v>
+      </c>
+      <c r="N7">
+        <v>3.45</v>
+      </c>
+      <c r="O7">
+        <v>3.84</v>
+      </c>
+      <c r="P7">
+        <v>3.36</v>
+      </c>
+      <c r="Q7">
+        <v>4.03</v>
+      </c>
+      <c r="R7">
+        <v>4.03</v>
+      </c>
+      <c r="S7">
+        <v>3.57</v>
+      </c>
+      <c r="T7">
+        <v>3.81</v>
+      </c>
+      <c r="U7">
+        <v>3.16</v>
+      </c>
+      <c r="V7">
+        <v>4.46</v>
+      </c>
+      <c r="W7">
+        <v>4</v>
+      </c>
+      <c r="X7">
+        <v>3.32</v>
+      </c>
+      <c r="Y7">
+        <v>2.63</v>
+      </c>
+      <c r="Z7">
+        <v>4.72</v>
+      </c>
+      <c r="AA7">
+        <v>6.99</v>
+      </c>
+      <c r="AB7">
+        <v>4.08</v>
+      </c>
+      <c r="AC7">
+        <v>3.75</v>
+      </c>
+      <c r="AD7">
+        <v>3.26</v>
+      </c>
+      <c r="AE7">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="AF7">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="AG7">
+        <v>3.64</v>
+      </c>
+      <c r="AH7">
+        <v>3.2</v>
+      </c>
+      <c r="AI7">
+        <v>5.4</v>
+      </c>
+      <c r="AJ7">
+        <v>6.39</v>
+      </c>
+      <c r="AK7">
+        <v>4.42</v>
+      </c>
+      <c r="AL7">
+        <v>5.81</v>
+      </c>
+      <c r="AM7">
+        <v>7.13</v>
+      </c>
+      <c r="AN7">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="AO7">
+        <v>6.92</v>
+      </c>
+      <c r="AP7">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="AQ7">
+        <v>6.99</v>
+      </c>
+      <c r="AR7">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="AS7">
+        <v>6.56</v>
+      </c>
+      <c r="AT7">
+        <v>9.57</v>
+      </c>
+      <c r="AU7">
+        <v>7.58</v>
+      </c>
+      <c r="AV7">
+        <v>6.87</v>
+      </c>
+      <c r="AW7">
+        <v>5</v>
+      </c>
+      <c r="AX7">
+        <v>6.81</v>
+      </c>
+      <c r="AY7">
+        <v>4.68</v>
+      </c>
+      <c r="AZ7">
+        <v>5.89</v>
+      </c>
+      <c r="BA7">
+        <v>5.94</v>
+      </c>
+      <c r="BB7">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54">
+      <c r="C8" s="7">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>1.48</v>
+      </c>
+      <c r="F8">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="G8">
+        <v>4.72</v>
+      </c>
+      <c r="H8">
+        <v>5.98</v>
+      </c>
+      <c r="I8">
+        <v>5.36</v>
+      </c>
+      <c r="J8">
+        <v>5.74</v>
+      </c>
+      <c r="K8">
+        <v>5.66</v>
+      </c>
+      <c r="L8">
+        <v>5.72</v>
+      </c>
+      <c r="M8">
+        <v>5.58</v>
+      </c>
+      <c r="N8">
+        <v>5.23</v>
+      </c>
+      <c r="O8">
+        <v>5.58</v>
+      </c>
+      <c r="P8">
+        <v>5.22</v>
+      </c>
+      <c r="Q8">
+        <v>5.66</v>
+      </c>
+      <c r="R8">
+        <v>5.58</v>
+      </c>
+      <c r="S8">
+        <v>5.44</v>
+      </c>
+      <c r="T8">
+        <v>5.41</v>
+      </c>
+      <c r="U8">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="V8">
+        <v>5.72</v>
+      </c>
+      <c r="W8">
+        <v>5.37</v>
+      </c>
+      <c r="X8">
+        <v>5.01</v>
+      </c>
+      <c r="Y8">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="Z8">
+        <v>5.63</v>
+      </c>
+      <c r="AA8">
+        <v>6.13</v>
+      </c>
+      <c r="AB8">
+        <v>5.42</v>
+      </c>
+      <c r="AC8">
+        <v>5.22</v>
+      </c>
+      <c r="AD8">
+        <v>5.04</v>
+      </c>
+      <c r="AE8">
+        <v>5.44</v>
+      </c>
+      <c r="AF8">
+        <v>5.45</v>
+      </c>
+      <c r="AG8">
+        <v>5.15</v>
+      </c>
+      <c r="AH8">
+        <v>4.97</v>
+      </c>
+      <c r="AI8">
+        <v>4.26</v>
+      </c>
+      <c r="AJ8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AK8">
+        <v>4</v>
+      </c>
+      <c r="AL8">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="AM8">
+        <v>5.12</v>
+      </c>
+      <c r="AN8">
+        <v>4.75</v>
+      </c>
+      <c r="AO8">
+        <v>5.31</v>
+      </c>
+      <c r="AP8">
+        <v>5.56</v>
+      </c>
+      <c r="AQ8">
+        <v>5.27</v>
+      </c>
+      <c r="AR8">
+        <v>4.46</v>
+      </c>
+      <c r="AS8">
+        <v>6.2</v>
+      </c>
+      <c r="AT8">
+        <v>6.49</v>
+      </c>
+      <c r="AU8">
+        <v>6.32</v>
+      </c>
+      <c r="AV8">
+        <v>6.16</v>
+      </c>
+      <c r="AW8">
+        <v>5.68</v>
+      </c>
+      <c r="AX8">
+        <v>5.94</v>
+      </c>
+      <c r="AY8">
+        <v>5.37</v>
+      </c>
+      <c r="AZ8">
+        <v>5.93</v>
+      </c>
+      <c r="BA8">
+        <v>5.76</v>
+      </c>
+      <c r="BB8">
+        <v>5.03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E9">
+        <v>29.4</v>
+      </c>
+      <c r="F9">
+        <v>6.6199999999999995E-2</v>
+      </c>
+      <c r="G9">
+        <v>1.84</v>
+      </c>
+      <c r="H9">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="I9">
+        <v>1.2</v>
+      </c>
+      <c r="J9">
+        <v>0.115</v>
+      </c>
+      <c r="K9">
+        <v>0.377</v>
+      </c>
+      <c r="L9">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="M9">
+        <v>2.85</v>
+      </c>
+      <c r="N9">
+        <v>3.17</v>
+      </c>
+      <c r="O9">
+        <v>2.59</v>
+      </c>
+      <c r="P9">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="Q9">
+        <v>1.41</v>
+      </c>
+      <c r="R9">
+        <v>5.68</v>
+      </c>
+      <c r="S9">
+        <v>6.81</v>
+      </c>
+      <c r="T9">
+        <v>2.8</v>
+      </c>
+      <c r="U9">
+        <v>10.8</v>
+      </c>
+      <c r="V9">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="W9">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="X9">
+        <v>11.4</v>
+      </c>
+      <c r="Y9">
+        <v>31.7</v>
+      </c>
+      <c r="Z9">
+        <v>2.39</v>
+      </c>
+      <c r="AA9">
+        <v>20.7</v>
+      </c>
+      <c r="AB9">
+        <v>3.02</v>
+      </c>
+      <c r="AC9">
+        <v>9.15</v>
+      </c>
+      <c r="AD9">
+        <v>10.1</v>
+      </c>
+      <c r="AE9">
+        <v>2.17</v>
+      </c>
+      <c r="AF9">
+        <v>2.85</v>
+      </c>
+      <c r="AG9">
+        <v>9.9</v>
+      </c>
+      <c r="AH9">
+        <v>10.8</v>
+      </c>
+      <c r="AI9">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="AJ9">
+        <v>3.2</v>
+      </c>
+      <c r="AK9">
+        <v>6.31</v>
+      </c>
+      <c r="AL9">
+        <v>2.41</v>
+      </c>
+      <c r="AM9">
+        <v>5.84</v>
+      </c>
+      <c r="AN9">
+        <v>11.8</v>
+      </c>
+      <c r="AO9">
+        <v>1.35</v>
+      </c>
+      <c r="AP9">
+        <v>2.58</v>
+      </c>
+      <c r="AQ9">
+        <v>6.16</v>
+      </c>
+      <c r="AR9">
+        <v>21.9</v>
+      </c>
+      <c r="AS9">
+        <v>1.39</v>
+      </c>
+      <c r="AT9">
+        <v>2.72</v>
+      </c>
+      <c r="AU9">
+        <v>3.82</v>
+      </c>
+      <c r="AV9">
+        <v>5.44</v>
+      </c>
+      <c r="AW9">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="AX9">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="AY9">
+        <v>12.1</v>
+      </c>
+      <c r="AZ9">
+        <v>3.51</v>
+      </c>
+      <c r="BA9">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="BB9">
+        <v>27.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54">
+      <c r="C10" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="E10">
+        <v>10.7</v>
+      </c>
+      <c r="F10">
+        <v>0.128</v>
+      </c>
+      <c r="G10">
+        <v>1.52</v>
+      </c>
+      <c r="H10">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="I10">
+        <v>1.23</v>
+      </c>
+      <c r="J10">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="K10">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="L10">
+        <v>1.9</v>
+      </c>
+      <c r="M10">
+        <v>2.17</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <v>1.76</v>
+      </c>
+      <c r="P10">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="Q10">
+        <v>1.24</v>
+      </c>
+      <c r="R10">
+        <v>3.24</v>
+      </c>
+      <c r="S10">
+        <v>3.66</v>
+      </c>
+      <c r="T10">
+        <v>1.86</v>
+      </c>
+      <c r="U10">
+        <v>4.54</v>
+      </c>
+      <c r="V10">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="W10">
+        <v>1.67</v>
+      </c>
+      <c r="X10">
+        <v>4.87</v>
+      </c>
+      <c r="Y10">
+        <v>11.6</v>
+      </c>
+      <c r="Z10">
+        <v>1.68</v>
+      </c>
+      <c r="AA10">
+        <v>6.3</v>
+      </c>
+      <c r="AB10">
+        <v>1.93</v>
+      </c>
+      <c r="AC10">
+        <v>3.84</v>
+      </c>
+      <c r="AD10">
+        <v>4.12</v>
+      </c>
+      <c r="AE10">
+        <v>1.58</v>
+      </c>
+      <c r="AF10">
+        <v>1.82</v>
+      </c>
+      <c r="AG10">
+        <v>4</v>
+      </c>
+      <c r="AH10">
+        <v>4.16</v>
+      </c>
+      <c r="AI10">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="AJ10">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AK10">
+        <v>3.25</v>
+      </c>
+      <c r="AL10">
+        <v>2.94</v>
+      </c>
+      <c r="AM10">
+        <v>3.83</v>
+      </c>
+      <c r="AN10">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="AO10">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="AP10">
+        <v>2.92</v>
+      </c>
+      <c r="AQ10">
+        <v>3.63</v>
+      </c>
+      <c r="AR10">
+        <v>6.44</v>
+      </c>
+      <c r="AS10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AT10">
+        <v>3.09</v>
+      </c>
+      <c r="AU10">
+        <v>3.52</v>
+      </c>
+      <c r="AV10">
+        <v>4.05</v>
+      </c>
+      <c r="AW10">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="AX10">
+        <v>5.14</v>
+      </c>
+      <c r="AY10">
+        <v>5.75</v>
+      </c>
+      <c r="AZ10">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="BA10">
+        <v>5.21</v>
+      </c>
+      <c r="BB10">
+        <v>9.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>34</v>
+      </c>
+      <c r="G11">
+        <v>31.9</v>
+      </c>
+      <c r="L11">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="R11">
+        <v>35.5</v>
+      </c>
+      <c r="W11">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="X11">
+        <v>36.1</v>
+      </c>
+      <c r="Y11">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="Z11">
+        <v>28.3</v>
+      </c>
+      <c r="AD11">
+        <v>8.9</v>
+      </c>
+      <c r="AG11">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="AH11">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="AI11">
+        <v>30.3</v>
+      </c>
+      <c r="AJ11">
+        <v>34.1</v>
+      </c>
+      <c r="AK11">
+        <v>34.1</v>
+      </c>
+      <c r="AL11">
+        <v>33.6</v>
+      </c>
+      <c r="AM11">
+        <v>35</v>
+      </c>
+      <c r="AN11">
+        <v>35.1</v>
+      </c>
+      <c r="AO11">
+        <v>30</v>
+      </c>
+      <c r="AP11">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="AQ11">
+        <v>33.5</v>
+      </c>
+      <c r="AR11">
+        <v>35</v>
+      </c>
+      <c r="BB11">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54">
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12">
+        <v>1.9</v>
+      </c>
+      <c r="G12">
+        <v>1.2</v>
+      </c>
+      <c r="L12">
+        <v>0.43</v>
+      </c>
+      <c r="R12">
+        <v>0.38</v>
+      </c>
+      <c r="W12">
+        <v>0.35</v>
+      </c>
+      <c r="X12">
+        <v>0.38</v>
+      </c>
+      <c r="Y12">
+        <v>0.36</v>
+      </c>
+      <c r="Z12">
+        <v>0.79</v>
+      </c>
+      <c r="AD12">
+        <v>0.36</v>
+      </c>
+      <c r="AG12">
+        <v>0.44</v>
+      </c>
+      <c r="AH12">
+        <v>0.65</v>
+      </c>
+      <c r="AI12">
+        <v>0.77</v>
+      </c>
+      <c r="AJ12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AK12">
+        <v>0.78</v>
+      </c>
+      <c r="AL12">
+        <v>0.54</v>
+      </c>
+      <c r="AM12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AN12">
+        <v>0.7</v>
+      </c>
+      <c r="AO12">
+        <v>0.75</v>
+      </c>
+      <c r="AP12">
+        <v>1.5</v>
+      </c>
+      <c r="AQ12">
+        <v>1.2</v>
+      </c>
+      <c r="AR12">
+        <v>0.87</v>
+      </c>
+      <c r="BB12">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54">
+      <c r="F13">
+        <v>66.900000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54">
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:54">
+      <c r="A17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="6">
+        <v>22</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="G17">
+        <v>20</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <v>12</v>
+      </c>
+      <c r="J17">
+        <v>14</v>
+      </c>
+      <c r="K17">
+        <v>11</v>
+      </c>
+      <c r="N17">
+        <v>12</v>
+      </c>
+      <c r="O17">
+        <v>13</v>
+      </c>
+      <c r="Q17">
+        <v>13</v>
+      </c>
+      <c r="W17">
+        <v>12.5</v>
+      </c>
+      <c r="AB17">
+        <v>12.5</v>
+      </c>
+      <c r="AI17">
+        <v>10</v>
+      </c>
+      <c r="AS17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:54">
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6">
+        <v>70</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="H18">
+        <v>60</v>
+      </c>
+      <c r="I18">
+        <v>36</v>
+      </c>
+      <c r="J18">
+        <v>24</v>
+      </c>
+      <c r="K18">
+        <v>32</v>
+      </c>
+      <c r="O18">
+        <v>31</v>
+      </c>
+      <c r="Q18">
+        <v>32</v>
+      </c>
+      <c r="V18">
+        <v>33</v>
+      </c>
+      <c r="W18">
+        <v>45</v>
+      </c>
+      <c r="AB18">
+        <v>26</v>
+      </c>
+      <c r="AI18">
+        <v>30</v>
+      </c>
+      <c r="AS18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:54">
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="6">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>3.6</v>
+      </c>
+      <c r="J19">
+        <v>3.8</v>
+      </c>
+      <c r="K19">
+        <v>3.8</v>
+      </c>
+      <c r="N19">
+        <v>3.5</v>
+      </c>
+      <c r="O19">
+        <v>3.7</v>
+      </c>
+      <c r="Q19">
+        <v>3.6</v>
+      </c>
+      <c r="T19">
+        <v>3.5</v>
+      </c>
+      <c r="W19">
+        <v>3.3</v>
+      </c>
+      <c r="AF19">
+        <v>3.2</v>
+      </c>
+      <c r="AI19">
+        <v>2</v>
+      </c>
+      <c r="AL19">
+        <v>2.5</v>
+      </c>
+      <c r="AS19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:54">
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="AI20">
+        <v>0.3</v>
+      </c>
+      <c r="AL20">
+        <v>1</v>
+      </c>
+      <c r="AS20">
+        <v>1.2</v>
+      </c>
+      <c r="AW20">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:54">
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:54">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="D22" s="6">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="T22">
+        <f>D22*1.25</f>
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <v>1.6800000000000002</v>
+      </c>
+      <c r="AI22">
+        <f>D22*1.75</f>
+        <v>1.9600000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:54">
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="T23">
+        <f t="shared" ref="T23:T25" si="0">D23*1.25</f>
+        <v>0.75</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="AI23">
+        <f t="shared" ref="AI23:AI25" si="1">D23*1.75</f>
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:54">
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>0.152</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+      <c r="AF24">
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="AI24">
+        <f t="shared" si="1"/>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:54">
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="D25" s="6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="0"/>
+        <v>2.75</v>
+      </c>
+      <c r="AE25">
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="AI25">
+        <f t="shared" si="1"/>
+        <v>3.8500000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:54">
+      <c r="B26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="D26" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="F26">
+        <v>6.95</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="N26">
+        <v>4.5</v>
+      </c>
+      <c r="O26">
+        <v>4.25</v>
+      </c>
+      <c r="Q26">
+        <v>4</v>
+      </c>
+      <c r="T26">
+        <v>4.5</v>
+      </c>
+      <c r="AF26">
+        <v>5</v>
+      </c>
+      <c r="AI26">
+        <f>D26*2.4</f>
+        <v>6</v>
+      </c>
+      <c r="AS26">
+        <v>4.5</v>
+      </c>
+      <c r="AW26">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="AZ26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:54">
+      <c r="B27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1.65</v>
+      </c>
+      <c r="F27">
+        <v>4.58</v>
+      </c>
+      <c r="G27">
+        <v>3.3</v>
+      </c>
+      <c r="H27">
+        <v>2.64</v>
+      </c>
+      <c r="N27">
+        <v>2.97</v>
+      </c>
+      <c r="O27">
+        <v>2.8</v>
+      </c>
+      <c r="Q27">
+        <v>2.64</v>
+      </c>
+      <c r="T27">
+        <v>2.97</v>
+      </c>
+      <c r="AF27">
+        <v>3.3</v>
+      </c>
+      <c r="AI27">
+        <f>D27*2.4</f>
+        <v>3.9599999999999995</v>
+      </c>
+      <c r="AS27">
+        <v>2.97</v>
+      </c>
+      <c r="AW27">
+        <v>3.2</v>
+      </c>
+      <c r="AZ27">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:54">
+      <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="N28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="Q28">
+        <v>0.12</v>
+      </c>
+      <c r="T28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AI28">
+        <v>0.12</v>
+      </c>
+      <c r="AS28">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:54">
+      <c r="B29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29">
+        <v>0.11</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="N29">
+        <v>0.7</v>
+      </c>
+      <c r="Q29">
+        <v>0.6</v>
+      </c>
+      <c r="T29">
+        <v>0.7</v>
+      </c>
+      <c r="AI29">
+        <v>0.6</v>
+      </c>
+      <c r="AS29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:54">
+      <c r="B30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>1.79</v>
+      </c>
+      <c r="D30" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="F30">
+        <v>12.1</v>
+      </c>
+      <c r="I30" s="6">
+        <v>11.2</v>
+      </c>
+      <c r="Y30">
+        <v>0</v>
+      </c>
+      <c r="Z30">
+        <v>11.2</v>
+      </c>
+      <c r="AA30">
+        <v>6.4</v>
+      </c>
+      <c r="AB30" s="6">
+        <v>6.4</v>
+      </c>
+      <c r="AS30">
+        <v>3.2</v>
+      </c>
+      <c r="BB30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:54">
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>6.67</v>
+      </c>
+      <c r="D31" s="6">
+        <v>23</v>
+      </c>
+      <c r="F31">
+        <v>43.5</v>
+      </c>
+      <c r="I31" s="6">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="V31">
+        <v>33.6</v>
+      </c>
+      <c r="Y31">
+        <v>0</v>
+      </c>
+      <c r="Z31">
+        <v>33.6</v>
+      </c>
+      <c r="AA31">
+        <v>10.6</v>
+      </c>
+      <c r="AB31" s="6">
+        <v>10.6</v>
+      </c>
+      <c r="AF31">
+        <v>9.6</v>
+      </c>
+      <c r="AS31">
+        <v>5.3</v>
+      </c>
+      <c r="BB31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:54">
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32">
+        <v>0.68</v>
+      </c>
+      <c r="D32" s="6">
+        <v>2</v>
+      </c>
+      <c r="I32" s="6">
+        <v>2</v>
+      </c>
+      <c r="N32">
+        <v>1.5</v>
+      </c>
+      <c r="Q32">
+        <v>1.3</v>
+      </c>
+      <c r="T32">
+        <v>1.5</v>
+      </c>
+      <c r="V32">
+        <v>1.3</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="6">
+        <v>2</v>
+      </c>
+      <c r="AF32">
+        <v>1.3</v>
+      </c>
+      <c r="AL32">
+        <v>0.8</v>
+      </c>
+      <c r="AS32">
+        <v>0.4</v>
+      </c>
+      <c r="BA32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:54">
+      <c r="B33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="D33" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="I33" s="6">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T33">
+        <v>1.27</v>
+      </c>
+      <c r="V33">
+        <v>1.3</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="6">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="AF33">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AL33">
+        <v>1</v>
+      </c>
+      <c r="AS33">
+        <v>0.6</v>
+      </c>
+      <c r="BA33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:54">
+      <c r="B34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <v>1.87</v>
+      </c>
+      <c r="D34" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="F34">
+        <v>6.4</v>
+      </c>
+      <c r="N34">
+        <v>5</v>
+      </c>
+      <c r="AI34">
+        <v>4</v>
+      </c>
+      <c r="AO34">
+        <v>3</v>
+      </c>
+      <c r="AS34">
+        <v>2</v>
+      </c>
+      <c r="AZ34">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:54">
+      <c r="B35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>1.56</v>
+      </c>
+      <c r="D35" s="6">
+        <v>6</v>
+      </c>
+      <c r="F35">
+        <v>7</v>
+      </c>
+      <c r="G35">
+        <v>6</v>
+      </c>
+      <c r="O35">
+        <v>7</v>
+      </c>
+      <c r="Q35">
+        <v>8</v>
+      </c>
+      <c r="Y35">
+        <v>0</v>
+      </c>
+      <c r="Z35">
+        <v>8</v>
+      </c>
+      <c r="AI35">
+        <v>9</v>
+      </c>
+      <c r="AL35">
+        <v>10</v>
+      </c>
+      <c r="AO35">
+        <v>12</v>
+      </c>
+      <c r="BB35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:54">
+      <c r="B36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="D36" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="F36">
+        <v>1.4</v>
+      </c>
+      <c r="N36">
+        <v>1.2</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
+      <c r="AB36">
+        <v>1</v>
+      </c>
+      <c r="AO36">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:54">
+      <c r="B37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37">
+        <v>0.432</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0.92</v>
+      </c>
+      <c r="N37">
+        <v>0.8</v>
+      </c>
+      <c r="AO37">
+        <v>0.92</v>
+      </c>
+      <c r="AR37">
+        <v>0</v>
+      </c>
+      <c r="AS37">
+        <v>0.92</v>
+      </c>
+      <c r="AV37">
+        <v>0.3</v>
+      </c>
+      <c r="AW37">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:54">
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:54">
+      <c r="A39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1.7000000000000001E-4</v>
+      </c>
+      <c r="V39">
+        <v>1.2E-4</v>
+      </c>
+      <c r="W39">
+        <v>1E-4</v>
+      </c>
+      <c r="AI39">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="AW39">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:54">
+      <c r="B40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="6">
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="V40">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="AF40">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="AL40">
+        <v>1E-3</v>
+      </c>
+      <c r="AS40">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="AW40">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:54">
+      <c r="A42" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:54">
+      <c r="B43" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:54">
+      <c r="B44" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:54">
+      <c r="B45" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:54">
+      <c r="A46" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:54">
+      <c r="B47" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:54">
+      <c r="B48" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="B49" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="B54" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:CV58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E15" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="10.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.25" customWidth="1"/>
     <col min="4" max="4" width="9" style="6"/>
     <col min="6" max="7" width="9" style="4"/>
     <col min="8" max="8" width="9" style="4" customWidth="1"/>

</xml_diff>

<commit_message>
Double number of short bursts per stimulus cycle. Enable multi-round stimulus per cycle for each assembly in short burst stimulus.
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="337">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1284,6 +1284,86 @@
   </si>
   <si>
     <t>input firing rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_51</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_52</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_53</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_53</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_53</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decrease thalamus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>from 50 to 40 Hz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set thalamus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>back to 50 Hz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_52</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_52</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_54</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short_54</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>duration by half</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>decrease short burst</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1794,13 +1874,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:FO46"/>
+  <dimension ref="A1:GE46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="FH3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="FV27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="FO17" sqref="FO17"/>
+      <selection pane="bottomRight" activeCell="GD44" sqref="GD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1811,9 +1891,11 @@
     <col min="80" max="85" width="9" style="4"/>
     <col min="116" max="116" width="9" style="14"/>
     <col min="168" max="170" width="9" style="13"/>
+    <col min="178" max="181" width="9" style="4"/>
+    <col min="183" max="183" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:171">
+    <row r="1" spans="1:187">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2302,8 +2384,50 @@
       <c r="FN1" s="13" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="2" spans="1:171">
+      <c r="FO1" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="FP1" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="FQ1" t="s">
+        <v>326</v>
+      </c>
+      <c r="FR1" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="FS1" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="FT1" t="s">
+        <v>322</v>
+      </c>
+      <c r="FV1" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="FW1" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="FX1" t="s">
+        <v>319</v>
+      </c>
+      <c r="FY1" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="FZ1" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="GA1" t="s">
+        <v>332</v>
+      </c>
+      <c r="GD1" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="GE1" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="2" spans="1:187">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -2312,7 +2436,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:171">
+    <row r="3" spans="1:187">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2811,11 +2935,56 @@
       <c r="FN3" s="13">
         <v>1.1299999999999999</v>
       </c>
-      <c r="FO3" s="7">
+      <c r="FO3">
+        <v>1.79</v>
+      </c>
+      <c r="FP3">
+        <v>2.68</v>
+      </c>
+      <c r="FQ3">
+        <v>1.36</v>
+      </c>
+      <c r="FR3">
+        <v>1.76</v>
+      </c>
+      <c r="FS3">
+        <v>2.77</v>
+      </c>
+      <c r="FT3">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="FU3" s="7">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="4" spans="1:171">
+      <c r="FV3" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="FW3" s="4">
+        <v>2.66</v>
+      </c>
+      <c r="FX3" s="4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="FY3" s="4">
+        <v>1.73</v>
+      </c>
+      <c r="FZ3" s="4">
+        <v>2.79</v>
+      </c>
+      <c r="GA3" s="4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="GC3" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="GD3">
+        <v>1.84</v>
+      </c>
+      <c r="GE3">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:187">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -3312,11 +3481,56 @@
       <c r="FN4" s="13">
         <v>0.94899999999999995</v>
       </c>
-      <c r="FO4" s="7">
+      <c r="FO4">
+        <v>1.42</v>
+      </c>
+      <c r="FP4">
+        <v>1.55</v>
+      </c>
+      <c r="FQ4">
+        <v>1.04</v>
+      </c>
+      <c r="FR4">
+        <v>1.41</v>
+      </c>
+      <c r="FS4">
+        <v>1.45</v>
+      </c>
+      <c r="FT4">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="FU4" s="7">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:171">
+      <c r="FV4" s="4">
+        <v>1.39</v>
+      </c>
+      <c r="FW4" s="4">
+        <v>1.44</v>
+      </c>
+      <c r="FX4" s="4">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="FY4" s="4">
+        <v>1.41</v>
+      </c>
+      <c r="FZ4" s="4">
+        <v>1.46</v>
+      </c>
+      <c r="GA4" s="4">
+        <v>0.873</v>
+      </c>
+      <c r="GC4" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="GD4">
+        <v>1.43</v>
+      </c>
+      <c r="GE4">
+        <v>1.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:187">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -3813,11 +4027,56 @@
       <c r="FN5" s="13">
         <v>2.2000000000000002</v>
       </c>
-      <c r="FO5" s="7">
+      <c r="FO5">
+        <v>1.45</v>
+      </c>
+      <c r="FP5">
+        <v>1.53</v>
+      </c>
+      <c r="FQ5">
+        <v>2.02</v>
+      </c>
+      <c r="FR5">
+        <v>1.45</v>
+      </c>
+      <c r="FS5">
+        <v>1.72</v>
+      </c>
+      <c r="FT5">
+        <v>2.33</v>
+      </c>
+      <c r="FU5" s="7">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:171">
+      <c r="FV5" s="4">
+        <v>1.52</v>
+      </c>
+      <c r="FW5" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="FX5" s="4">
+        <v>2.37</v>
+      </c>
+      <c r="FY5" s="4">
+        <v>1.51</v>
+      </c>
+      <c r="FZ5" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="GA5" s="4">
+        <v>2.41</v>
+      </c>
+      <c r="GC5" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="GD5">
+        <v>1.43</v>
+      </c>
+      <c r="GE5">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:187">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="7">
@@ -4312,11 +4571,56 @@
       <c r="FN6" s="13">
         <v>1.37</v>
       </c>
-      <c r="FO6" s="7">
+      <c r="FO6">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="FP6">
+        <v>1.07</v>
+      </c>
+      <c r="FQ6">
+        <v>1.29</v>
+      </c>
+      <c r="FR6">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="FS6">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="FT6">
+        <v>1.4</v>
+      </c>
+      <c r="FU6" s="7">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:171">
+      <c r="FV6" s="4">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="FW6" s="4">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="FX6" s="4">
+        <v>1.43</v>
+      </c>
+      <c r="FY6" s="4">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="FZ6" s="4">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="GA6" s="4">
+        <v>1.44</v>
+      </c>
+      <c r="GC6" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="GD6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="GE6">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:187">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -4813,11 +5117,56 @@
       <c r="FN7" s="13">
         <v>5.38</v>
       </c>
-      <c r="FO7" s="7">
+      <c r="FO7">
+        <v>7.43</v>
+      </c>
+      <c r="FP7">
+        <v>10.1</v>
+      </c>
+      <c r="FQ7">
+        <v>6.13</v>
+      </c>
+      <c r="FR7">
+        <v>7.4</v>
+      </c>
+      <c r="FS7">
+        <v>10.4</v>
+      </c>
+      <c r="FT7">
+        <v>5.2</v>
+      </c>
+      <c r="FU7" s="7">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:171">
+      <c r="FV7" s="4">
+        <v>7.63</v>
+      </c>
+      <c r="FW7" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="FX7" s="4">
+        <v>5.57</v>
+      </c>
+      <c r="FY7" s="4">
+        <v>7.61</v>
+      </c>
+      <c r="FZ7" s="4">
+        <v>10.9</v>
+      </c>
+      <c r="GA7" s="4">
+        <v>5.41</v>
+      </c>
+      <c r="GC7" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="GD7">
+        <v>7.56</v>
+      </c>
+      <c r="GE7">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:187">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="7">
@@ -5312,11 +5661,56 @@
       <c r="FN8" s="13">
         <v>5.82</v>
       </c>
-      <c r="FO8" s="7">
+      <c r="FO8">
+        <v>6.2</v>
+      </c>
+      <c r="FP8">
+        <v>6.43</v>
+      </c>
+      <c r="FQ8">
+        <v>5.92</v>
+      </c>
+      <c r="FR8">
+        <v>6.17</v>
+      </c>
+      <c r="FS8">
+        <v>6.43</v>
+      </c>
+      <c r="FT8">
+        <v>5.69</v>
+      </c>
+      <c r="FU8" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:171">
+      <c r="FV8" s="4">
+        <v>6.36</v>
+      </c>
+      <c r="FW8" s="4">
+        <v>6.52</v>
+      </c>
+      <c r="FX8" s="4">
+        <v>5.84</v>
+      </c>
+      <c r="FY8" s="4">
+        <v>6.15</v>
+      </c>
+      <c r="FZ8" s="4">
+        <v>6.43</v>
+      </c>
+      <c r="GA8" s="4">
+        <v>5.62</v>
+      </c>
+      <c r="GC8" s="7">
+        <v>6</v>
+      </c>
+      <c r="GD8">
+        <v>6.19</v>
+      </c>
+      <c r="GE8">
+        <v>6.66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:187">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -5813,11 +6207,56 @@
       <c r="FN9" s="13">
         <v>13.9</v>
       </c>
-      <c r="FO9" s="7">
+      <c r="FO9">
+        <v>3.53</v>
+      </c>
+      <c r="FP9">
+        <v>3.93</v>
+      </c>
+      <c r="FQ9">
+        <v>9.86</v>
+      </c>
+      <c r="FR9">
+        <v>3.52</v>
+      </c>
+      <c r="FS9">
+        <v>5.07</v>
+      </c>
+      <c r="FT9">
+        <v>18</v>
+      </c>
+      <c r="FU9" s="7">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:171">
+      <c r="FV9" s="4">
+        <v>3.49</v>
+      </c>
+      <c r="FW9" s="4">
+        <v>5.34</v>
+      </c>
+      <c r="FX9" s="4">
+        <v>18.3</v>
+      </c>
+      <c r="FY9" s="4">
+        <v>3.44</v>
+      </c>
+      <c r="FZ9" s="4">
+        <v>4.92</v>
+      </c>
+      <c r="GA9" s="4">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="GC9" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="GD9">
+        <v>3.44</v>
+      </c>
+      <c r="GE9">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:187">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="7">
@@ -6312,11 +6751,56 @@
       <c r="FN10" s="13">
         <v>6.56</v>
       </c>
-      <c r="FO10" s="7">
+      <c r="FO10">
+        <v>4.09</v>
+      </c>
+      <c r="FP10">
+        <v>4.2</v>
+      </c>
+      <c r="FQ10">
+        <v>5.52</v>
+      </c>
+      <c r="FR10">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="FS10">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="FT10">
+        <v>7.67</v>
+      </c>
+      <c r="FU10" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:171">
+      <c r="FV10" s="4">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="FW10" s="4">
+        <v>4.42</v>
+      </c>
+      <c r="FX10" s="4">
+        <v>7.75</v>
+      </c>
+      <c r="FY10" s="4">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="FZ10" s="4">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="GA10" s="4">
+        <v>7.76</v>
+      </c>
+      <c r="GC10" s="7">
+        <v>4</v>
+      </c>
+      <c r="GD10">
+        <v>4.12</v>
+      </c>
+      <c r="GE10">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:187">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -6679,8 +7163,33 @@
       <c r="FN11" s="13">
         <v>23.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:171">
+      <c r="FP11">
+        <v>31.3</v>
+      </c>
+      <c r="FQ11" s="4"/>
+      <c r="FS11">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="FT11" s="4">
+        <v>28</v>
+      </c>
+      <c r="FW11" s="4">
+        <v>36</v>
+      </c>
+      <c r="FX11" s="4">
+        <v>26</v>
+      </c>
+      <c r="FZ11" s="4">
+        <v>33.5</v>
+      </c>
+      <c r="GA11" s="4">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="GE11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:187">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>31</v>
@@ -7038,8 +7547,33 @@
       <c r="FN12" s="13">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="13" spans="1:171">
+      <c r="FP12">
+        <v>0.49</v>
+      </c>
+      <c r="FQ12" s="4"/>
+      <c r="FS12">
+        <v>0.52</v>
+      </c>
+      <c r="FT12" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="FW12" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="FX12" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="FZ12" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="GA12" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="GE12">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:187">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="H13">
@@ -7125,8 +7659,25 @@
       <c r="FF13" s="14">
         <v>45.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:171">
+      <c r="FP13">
+        <v>46.2</v>
+      </c>
+      <c r="FQ13" s="4"/>
+      <c r="FT13" s="4"/>
+      <c r="FW13" s="4">
+        <v>31.8</v>
+      </c>
+      <c r="FZ13" s="4">
+        <v>38</v>
+      </c>
+      <c r="GA13" s="4">
+        <v>31.7</v>
+      </c>
+      <c r="GE13">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:187">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="H14">
@@ -7211,8 +7762,23 @@
       <c r="FF14" s="14">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="15" spans="1:171">
+      <c r="FP14">
+        <v>0.21</v>
+      </c>
+      <c r="FW14" s="4">
+        <v>0.46</v>
+      </c>
+      <c r="FZ14" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="GA14" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="GE14">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:187">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="BR15">
@@ -7220,7 +7786,7 @@
       </c>
       <c r="CE15"/>
     </row>
-    <row r="16" spans="1:171">
+    <row r="16" spans="1:187">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="BR16">
@@ -7228,7 +7794,7 @@
       </c>
       <c r="CE16"/>
     </row>
-    <row r="17" spans="1:168">
+    <row r="17" spans="1:186">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -7370,8 +7936,23 @@
       <c r="FL17" s="13">
         <v>12.8</v>
       </c>
-    </row>
-    <row r="18" spans="1:168">
+      <c r="FO17">
+        <v>12.8</v>
+      </c>
+      <c r="FR17">
+        <v>12.7</v>
+      </c>
+      <c r="FV17" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="GB17">
+        <v>12.45</v>
+      </c>
+      <c r="GD17" s="4">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:186">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
         <v>5</v>
@@ -7505,8 +8086,14 @@
       <c r="FL18" s="13">
         <v>81</v>
       </c>
-    </row>
-    <row r="19" spans="1:168">
+      <c r="FV18" s="4">
+        <v>84</v>
+      </c>
+      <c r="GD18" s="4">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:186">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
         <v>6</v>
@@ -7572,8 +8159,17 @@
       <c r="FL19" s="13">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:168">
+      <c r="FV19" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="FY19" s="4">
+        <v>3.23</v>
+      </c>
+      <c r="GD19" s="4">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:186">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>7</v>
@@ -7656,8 +8252,17 @@
       <c r="FL20" s="13">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="21" spans="1:168">
+      <c r="FV20" s="4">
+        <v>2.35</v>
+      </c>
+      <c r="FY20" s="4">
+        <v>2.38</v>
+      </c>
+      <c r="GD20" s="4">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:186">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
@@ -7672,8 +8277,9 @@
       <c r="G21" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="22" spans="1:168">
+      <c r="GD21" s="4"/>
+    </row>
+    <row r="22" spans="1:186">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -7702,8 +8308,11 @@
       <c r="FL22" s="13">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="23" spans="1:168">
+      <c r="GD22" s="4">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:186">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
         <v>13</v>
@@ -7731,8 +8340,11 @@
       <c r="FL23" s="13">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="24" spans="1:168">
+      <c r="GD23" s="4">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:186">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
         <v>15</v>
@@ -7760,8 +8372,11 @@
       <c r="FL24" s="13">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="25" spans="1:168">
+      <c r="GD24" s="4">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:186">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
         <v>14</v>
@@ -7789,8 +8404,11 @@
       <c r="FL25" s="13">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:168">
+      <c r="GD25" s="4">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:186">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
         <v>16</v>
@@ -7895,8 +8513,14 @@
       <c r="FL26" s="13">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="27" spans="1:168">
+      <c r="FY26" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="GD26" s="4">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:186">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
         <v>17</v>
@@ -8002,8 +8626,14 @@
       <c r="FL27" s="13">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="28" spans="1:168">
+      <c r="FY27" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="GD27" s="4">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:186">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
         <v>18</v>
@@ -8099,8 +8729,11 @@
       <c r="FL28" s="13">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="29" spans="1:168">
+      <c r="GD28" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:186">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
         <v>19</v>
@@ -8197,8 +8830,11 @@
       <c r="FL29" s="13">
         <v>6.2</v>
       </c>
-    </row>
-    <row r="30" spans="1:168">
+      <c r="GD29" s="4">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:186">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>20</v>
@@ -8243,11 +8879,17 @@
       <c r="CK30">
         <v>0.6</v>
       </c>
-      <c r="FH30" s="14">
+      <c r="FH30" s="4">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="31" spans="1:168">
+      <c r="FL30" s="13">
+        <v>0.63</v>
+      </c>
+      <c r="GD30" s="4">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:186">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
         <v>21</v>
@@ -8337,11 +8979,15 @@
       <c r="EP31">
         <v>9.4</v>
       </c>
-      <c r="FH31" s="14">
+      <c r="FH31" s="4"/>
+      <c r="FL31" s="13">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="32" spans="1:168">
+      <c r="GD31" s="4">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:186">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
         <v>22</v>
@@ -8438,8 +9084,11 @@
       <c r="FL32" s="13">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="33" spans="1:171">
+      <c r="GD32" s="4">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:187">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
         <v>30</v>
@@ -8536,8 +9185,11 @@
       <c r="FL33" s="13">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:171">
+      <c r="GD33" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:187">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
         <v>23</v>
@@ -8608,8 +9260,14 @@
       <c r="FL34" s="13">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="35" spans="1:171">
+      <c r="FY34" s="4">
+        <v>1</v>
+      </c>
+      <c r="GD34" s="4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:187">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
         <v>25</v>
@@ -8692,8 +9350,14 @@
       <c r="FL35" s="13">
         <v>22</v>
       </c>
-    </row>
-    <row r="36" spans="1:171">
+      <c r="GB35">
+        <v>24</v>
+      </c>
+      <c r="GD35" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:187">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
         <v>26</v>
@@ -8821,8 +9485,14 @@
       <c r="FL36" s="13">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="37" spans="1:171">
+      <c r="GB36">
+        <v>0.42</v>
+      </c>
+      <c r="GD36" s="4">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:187">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
         <v>24</v>
@@ -8899,8 +9569,17 @@
       <c r="FL37" s="13">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="38" spans="1:171">
+      <c r="FY37" s="4">
+        <v>2</v>
+      </c>
+      <c r="GB37">
+        <v>2.4</v>
+      </c>
+      <c r="GD37" s="4">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:187">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" t="s">
@@ -8916,7 +9595,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:171">
+    <row r="39" spans="1:187">
       <c r="F39" s="17">
         <v>7.4</v>
       </c>
@@ -8924,7 +9603,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="40" spans="1:171">
+    <row r="40" spans="1:187">
       <c r="A40" s="2" t="s">
         <v>35</v>
       </c>
@@ -8985,8 +9664,11 @@
       <c r="FL40" s="13">
         <v>1.7000000000000001E-4</v>
       </c>
-    </row>
-    <row r="41" spans="1:171">
+      <c r="GD40" s="4">
+        <v>1.7000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:187">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
         <v>24</v>
@@ -9057,35 +9739,65 @@
       <c r="FL41" s="13">
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:171">
+      <c r="GD41" s="4">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:187">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
     </row>
-    <row r="43" spans="1:171">
+    <row r="43" spans="1:187">
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:171">
+    <row r="44" spans="1:187">
       <c r="A44" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B44" s="2"/>
       <c r="FO44" t="s">
+        <v>327</v>
+      </c>
+      <c r="FR44" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="45" spans="1:171">
+      <c r="FT44" s="4"/>
+      <c r="GC44" t="s">
+        <v>329</v>
+      </c>
+      <c r="GE44" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="45" spans="1:187">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="FO45" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="46" spans="1:171">
+      <c r="FR45" t="s">
+        <v>316</v>
+      </c>
+      <c r="FT45" s="4"/>
+      <c r="GC45" t="s">
+        <v>316</v>
+      </c>
+      <c r="GE45" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="46" spans="1:187">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="FO46" t="s">
+        <v>328</v>
+      </c>
+      <c r="FR46" t="s">
         <v>314</v>
+      </c>
+      <c r="FT46" s="4"/>
+      <c r="GC46" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CS cell model
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -7,18 +7,19 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="7275"/>
   </bookViews>
   <sheets>
-    <sheet name="constrain postsyn CP CS ratio" sheetId="8" r:id="rId1"/>
-    <sheet name="init as M1" sheetId="6" r:id="rId2"/>
-    <sheet name="new set" sheetId="7" r:id="rId3"/>
-    <sheet name="set 2" sheetId="5" r:id="rId4"/>
-    <sheet name="set 1" sheetId="3" r:id="rId5"/>
+    <sheet name="new PN model" sheetId="9" r:id="rId1"/>
+    <sheet name="constrain postsyn CP CS ratio" sheetId="8" r:id="rId2"/>
+    <sheet name="init as M1" sheetId="6" r:id="rId3"/>
+    <sheet name="new set" sheetId="7" r:id="rId4"/>
+    <sheet name="set 2" sheetId="5" r:id="rId5"/>
+    <sheet name="set 1" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="340">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1364,6 +1365,18 @@
   </si>
   <si>
     <t>decrease short burst</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tune CP, CS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>single cell model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>passive properties</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1874,13 +1887,846 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="M21" sqref="M21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="5" max="5" width="9" style="6"/>
+    <col min="8" max="10" width="9" style="13"/>
+    <col min="12" max="12" width="9" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="H1" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="H3" s="13">
+        <v>1.81</v>
+      </c>
+      <c r="I3" s="13">
+        <v>2.8</v>
+      </c>
+      <c r="J3" s="13">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="K3">
+        <v>0.105</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="H4" s="13">
+        <v>1.42</v>
+      </c>
+      <c r="I4" s="13">
+        <v>1.51</v>
+      </c>
+      <c r="J4" s="13">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="K4">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="H5" s="13">
+        <v>1.43</v>
+      </c>
+      <c r="I5" s="13">
+        <v>1.6</v>
+      </c>
+      <c r="J5" s="13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K5">
+        <v>2.75</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H6" s="13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I6" s="13">
+        <v>1.07</v>
+      </c>
+      <c r="J6" s="13">
+        <v>1.37</v>
+      </c>
+      <c r="K6">
+        <v>1.98</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7">
+        <v>5</v>
+      </c>
+      <c r="G7" s="7">
+        <v>7.5</v>
+      </c>
+      <c r="H7" s="13">
+        <v>7.5</v>
+      </c>
+      <c r="I7" s="13">
+        <v>10.4</v>
+      </c>
+      <c r="J7" s="13">
+        <v>5.38</v>
+      </c>
+      <c r="K7">
+        <v>4.53</v>
+      </c>
+      <c r="L7" s="4">
+        <v>6.62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="7">
+        <v>4</v>
+      </c>
+      <c r="G8" s="7">
+        <v>6</v>
+      </c>
+      <c r="H8" s="13">
+        <v>6.25</v>
+      </c>
+      <c r="I8" s="13">
+        <v>6.45</v>
+      </c>
+      <c r="J8" s="13">
+        <v>5.82</v>
+      </c>
+      <c r="K8">
+        <v>5.68</v>
+      </c>
+      <c r="L8" s="4">
+        <v>5.97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="H9" s="13">
+        <v>3.47</v>
+      </c>
+      <c r="I9" s="13">
+        <v>4.37</v>
+      </c>
+      <c r="J9" s="13">
+        <v>13.9</v>
+      </c>
+      <c r="K9">
+        <v>11.9</v>
+      </c>
+      <c r="L9" s="4">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="G10" s="7">
+        <v>4</v>
+      </c>
+      <c r="H10" s="13">
+        <v>4.05</v>
+      </c>
+      <c r="I10" s="13">
+        <v>4.26</v>
+      </c>
+      <c r="J10" s="13">
+        <v>6.56</v>
+      </c>
+      <c r="K10">
+        <v>6.61</v>
+      </c>
+      <c r="L10" s="4">
+        <v>4.3899999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="13">
+        <v>31.9</v>
+      </c>
+      <c r="J11" s="13">
+        <v>23.1</v>
+      </c>
+      <c r="K11">
+        <v>14.1</v>
+      </c>
+      <c r="L11" s="4">
+        <v>29.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="13">
+        <v>0.38</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0.36</v>
+      </c>
+      <c r="K12">
+        <v>0.35</v>
+      </c>
+      <c r="L12" s="4">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="6">
+        <v>22</v>
+      </c>
+      <c r="H17" s="13">
+        <v>12.8</v>
+      </c>
+      <c r="L17" s="4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="6">
+        <v>70</v>
+      </c>
+      <c r="H18" s="13">
+        <v>81</v>
+      </c>
+      <c r="L18" s="4">
+        <v>52</v>
+      </c>
+      <c r="M18">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="6">
+        <v>3</v>
+      </c>
+      <c r="H19" s="13">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="H20" s="13">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" t="s">
+        <v>215</v>
+      </c>
+      <c r="G21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>0.25</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.78</v>
+      </c>
+      <c r="F22" s="17">
+        <v>1</v>
+      </c>
+      <c r="G22" s="4">
+        <f>ROUND(E22*F22,3)</f>
+        <v>0.78</v>
+      </c>
+      <c r="H22" s="13">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="E23" s="6">
+        <v>0.42</v>
+      </c>
+      <c r="F23">
+        <f>F$22</f>
+        <v>1</v>
+      </c>
+      <c r="G23" s="4">
+        <f t="shared" ref="G23:G33" si="0">ROUND(E23*F23,2)</f>
+        <v>0.42</v>
+      </c>
+      <c r="H23" s="13">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>0.156</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0.52</v>
+      </c>
+      <c r="F24">
+        <f>F$22</f>
+        <v>1</v>
+      </c>
+      <c r="G24" s="4">
+        <f t="shared" si="0"/>
+        <v>0.52</v>
+      </c>
+      <c r="H24" s="13">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <v>0.224</v>
+      </c>
+      <c r="E25" s="6">
+        <v>1.6</v>
+      </c>
+      <c r="F25">
+        <f>F$22</f>
+        <v>1</v>
+      </c>
+      <c r="G25" s="4">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="H25" s="13">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1.9</v>
+      </c>
+      <c r="F26" s="17">
+        <v>1.8</v>
+      </c>
+      <c r="G26" s="16">
+        <f t="shared" si="0"/>
+        <v>3.42</v>
+      </c>
+      <c r="H26" s="13">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27">
+        <v>0.4</v>
+      </c>
+      <c r="D27">
+        <v>0.36</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f>F$26*F$38</f>
+        <v>1.8</v>
+      </c>
+      <c r="G27" s="16">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
+      <c r="H27" s="13">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1.43</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0.08</v>
+      </c>
+      <c r="F28" s="17">
+        <v>7.29</v>
+      </c>
+      <c r="G28" s="15">
+        <f t="shared" si="0"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H28" s="13">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D29">
+        <v>0.2</v>
+      </c>
+      <c r="E29" s="6">
+        <v>0.85</v>
+      </c>
+      <c r="F29">
+        <f>F$28*F$38</f>
+        <v>7.29</v>
+      </c>
+      <c r="G29" s="15">
+        <f t="shared" si="0"/>
+        <v>6.2</v>
+      </c>
+      <c r="H29" s="13">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="D30">
+        <v>3.9</v>
+      </c>
+      <c r="E30" s="6">
+        <v>3.9</v>
+      </c>
+      <c r="F30" s="17">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="G30" s="14">
+        <f t="shared" si="0"/>
+        <v>0.63</v>
+      </c>
+      <c r="H30" s="13">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>6.4</v>
+      </c>
+      <c r="D31" s="7">
+        <v>3</v>
+      </c>
+      <c r="E31" s="6">
+        <v>16</v>
+      </c>
+      <c r="F31" s="17">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="G31" s="18">
+        <f>ROUND(E31*F31,2)</f>
+        <v>9.41</v>
+      </c>
+      <c r="H31" s="13">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="D32" s="7">
+        <v>12.6</v>
+      </c>
+      <c r="E32" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="F32">
+        <f>F$30*F$39</f>
+        <v>1.1988000000000001</v>
+      </c>
+      <c r="G32" s="14">
+        <f>ROUND(E32*F32,2)</f>
+        <v>2.1</v>
+      </c>
+      <c r="H32" s="13">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="D33">
+        <v>10.029999999999999</v>
+      </c>
+      <c r="E33" s="6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F33">
+        <f>F$31*F$39</f>
+        <v>4.3512000000000004</v>
+      </c>
+      <c r="G33" s="18">
+        <f t="shared" si="0"/>
+        <v>10.01</v>
+      </c>
+      <c r="H33" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <v>1.87</v>
+      </c>
+      <c r="E34" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="H34" s="13">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>1.57</v>
+      </c>
+      <c r="E35" s="6">
+        <v>3.65</v>
+      </c>
+      <c r="H35" s="13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="E36" s="6">
+        <v>2.4</v>
+      </c>
+      <c r="H36" s="13">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37">
+        <v>0.4</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="H37" s="13">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" s="17">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="F39" s="17">
+        <v>7.4</v>
+      </c>
+      <c r="G39" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="6">
+        <v>1.7000000000000001E-4</v>
+      </c>
+      <c r="H40" s="13">
+        <v>1.7000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="6">
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="H41" s="13">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="K44" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="K45" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="K46" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:GE46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="FV27" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="7" ySplit="2" topLeftCell="FX3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="GD44" sqref="GD44"/>
+      <selection pane="bottomRight" activeCell="GG1" sqref="GG1:GH1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -9807,12 +10653,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:ES58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
@@ -15967,7 +16813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DA58"/>
   <sheetViews>
@@ -20402,7 +21248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BB43"/>
   <sheetViews>
@@ -22766,7 +23612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CV56"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update new run results and figures
</commit_message>
<xml_diff>
--- a/Analysis/network_tuning.xlsx
+++ b/Analysis/network_tuning.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="320">
   <si>
     <t>Trial</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1275,16 +1275,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>from 50 to 60 Hz</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Increase thalamus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>input firing rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>New input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>random seed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>short</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>long_rand_single_assembly</t>
   </si>
 </sst>
 </file>
@@ -1794,13 +1805,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:FO46"/>
+  <dimension ref="A1:FW46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="2" topLeftCell="FH3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="FO17" sqref="FO17"/>
+      <selection pane="bottomRight" activeCell="FS17" sqref="FS17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1811,9 +1822,10 @@
     <col min="80" max="85" width="9" style="4"/>
     <col min="116" max="116" width="9" style="14"/>
     <col min="168" max="170" width="9" style="13"/>
+    <col min="172" max="175" width="9" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:171">
+    <row r="1" spans="1:179">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2302,8 +2314,24 @@
       <c r="FN1" s="13" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="2" spans="1:171">
+      <c r="FP1" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="FQ1" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="FR1" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="FS1" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="FT1" s="4"/>
+      <c r="FU1" s="4"/>
+      <c r="FV1" s="4"/>
+      <c r="FW1" s="4"/>
+    </row>
+    <row r="2" spans="1:179">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -2312,7 +2340,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:171">
+    <row r="3" spans="1:179">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2811,11 +2839,21 @@
       <c r="FN3" s="13">
         <v>1.1299999999999999</v>
       </c>
-      <c r="FO3" s="7">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:171">
+      <c r="FO3" s="4"/>
+      <c r="FP3" s="13">
+        <v>1.79</v>
+      </c>
+      <c r="FQ3" s="13">
+        <v>2.74</v>
+      </c>
+      <c r="FR3" s="13">
+        <v>1.19</v>
+      </c>
+      <c r="FS3" s="13">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:179">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -3312,11 +3350,21 @@
       <c r="FN4" s="13">
         <v>0.94899999999999995</v>
       </c>
-      <c r="FO4" s="7">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:171">
+      <c r="FO4" s="4"/>
+      <c r="FP4" s="13">
+        <v>1.42</v>
+      </c>
+      <c r="FQ4" s="13">
+        <v>1.49</v>
+      </c>
+      <c r="FR4" s="13">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="FS4" s="13">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:179">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -3813,11 +3861,21 @@
       <c r="FN5" s="13">
         <v>2.2000000000000002</v>
       </c>
-      <c r="FO5" s="7">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:171">
+      <c r="FO5" s="4"/>
+      <c r="FP5" s="13">
+        <v>1.45</v>
+      </c>
+      <c r="FQ5" s="13">
+        <v>1.63</v>
+      </c>
+      <c r="FR5" s="13">
+        <v>2.19</v>
+      </c>
+      <c r="FS5" s="13">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:179">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="7">
@@ -4312,11 +4370,21 @@
       <c r="FN6" s="13">
         <v>1.37</v>
       </c>
-      <c r="FO6" s="7">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:171">
+      <c r="FO6" s="4"/>
+      <c r="FP6" s="13">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="FQ6" s="13">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="FR6" s="13">
+        <v>1.37</v>
+      </c>
+      <c r="FS6" s="13">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:179">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -4813,11 +4881,21 @@
       <c r="FN7" s="13">
         <v>5.38</v>
       </c>
-      <c r="FO7" s="7">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:171">
+      <c r="FO7" s="4"/>
+      <c r="FP7" s="13">
+        <v>7.47</v>
+      </c>
+      <c r="FQ7" s="13">
+        <v>10.3</v>
+      </c>
+      <c r="FR7" s="13">
+        <v>5.55</v>
+      </c>
+      <c r="FS7" s="13">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:179">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="7">
@@ -5312,11 +5390,21 @@
       <c r="FN8" s="13">
         <v>5.82</v>
       </c>
-      <c r="FO8" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:171">
+      <c r="FO8" s="4"/>
+      <c r="FP8" s="13">
+        <v>6.21</v>
+      </c>
+      <c r="FQ8" s="13">
+        <v>6.42</v>
+      </c>
+      <c r="FR8" s="13">
+        <v>5.78</v>
+      </c>
+      <c r="FS8" s="13">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:179">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -5813,11 +5901,21 @@
       <c r="FN9" s="13">
         <v>13.9</v>
       </c>
-      <c r="FO9" s="7">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:171">
+      <c r="FO9" s="4"/>
+      <c r="FP9" s="13">
+        <v>3.52</v>
+      </c>
+      <c r="FQ9" s="13">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="FR9" s="13">
+        <v>13.9</v>
+      </c>
+      <c r="FS9" s="13">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:179">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="7">
@@ -6312,11 +6410,21 @@
       <c r="FN10" s="13">
         <v>6.56</v>
       </c>
-      <c r="FO10" s="7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:171">
+      <c r="FO10" s="4"/>
+      <c r="FP10" s="13">
+        <v>4.16</v>
+      </c>
+      <c r="FQ10" s="13">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="FR10" s="13">
+        <v>6.62</v>
+      </c>
+      <c r="FS10" s="13">
+        <v>7.39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:179">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -6679,8 +6787,15 @@
       <c r="FN11" s="13">
         <v>23.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:171">
+      <c r="FO11" s="4"/>
+      <c r="FQ11" s="13">
+        <v>33.9</v>
+      </c>
+      <c r="FS11" s="13">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:179">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>31</v>
@@ -7038,8 +7153,14 @@
       <c r="FN12" s="13">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="13" spans="1:171">
+      <c r="FQ12" s="13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="FS12" s="13">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:179">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="H13">
@@ -7126,7 +7247,7 @@
         <v>45.8</v>
       </c>
     </row>
-    <row r="14" spans="1:171">
+    <row r="14" spans="1:179">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="H14">
@@ -7212,7 +7333,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="15" spans="1:171">
+    <row r="15" spans="1:179">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="BR15">
@@ -7220,7 +7341,7 @@
       </c>
       <c r="CE15"/>
     </row>
-    <row r="16" spans="1:171">
+    <row r="16" spans="1:179">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="BR16">
@@ -9071,22 +9192,19 @@
       </c>
       <c r="B44" s="2"/>
       <c r="FO44" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="45" spans="1:171">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="FO45" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="46" spans="1:171">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
-      <c r="FO46" t="s">
-        <v>314</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>